<commit_message>
Starting to update support for desalting
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFAFB0B-A2D6-4A34-BCB3-B85FF5C79C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03309A35-0BA3-4F54-9567-B9EF893E3C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="90">
   <si>
     <t>Step</t>
   </si>
@@ -189,18 +189,12 @@
     <t>Shake (rpm)</t>
   </si>
   <si>
-    <t>Desalt</t>
-  </si>
-  <si>
     <t>7AA534</t>
   </si>
   <si>
     <t>Equilibration Buffer</t>
   </si>
   <si>
-    <t>SizeX:100,SizeX:100;SizeX:100</t>
-  </si>
-  <si>
     <t>Vacuum</t>
   </si>
   <si>
@@ -301,6 +295,15 @@
   </si>
   <si>
     <t>Supported?</t>
+  </si>
+  <si>
+    <t>Waste Plate</t>
+  </si>
+  <si>
+    <t>IMCS SizeX Desalt</t>
+  </si>
+  <si>
+    <t>100,200</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -434,6 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,10 +846,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:D296"/>
+  <dimension ref="B1:D301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +889,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -1001,7 +1005,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -1155,7 +1159,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" t="b">
         <v>1</v>
@@ -1227,7 +1231,9 @@
       <c r="B49" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="7"/>
+      <c r="C49" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
@@ -1269,7 +1275,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C55" t="b">
         <v>1</v>
@@ -1311,7 +1317,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C61" t="b">
         <v>1</v>
@@ -1485,7 +1491,7 @@
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D83" s="5"/>
     </row>
@@ -1548,7 +1554,7 @@
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C91" t="b">
         <v>1</v>
@@ -1784,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D123" s="3"/>
     </row>
@@ -1808,7 +1814,7 @@
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C126" t="b">
         <v>1</v>
@@ -1940,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="D143" s="3"/>
     </row>
@@ -1958,13 +1964,13 @@
         <v>3</v>
       </c>
       <c r="C145" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D145" s="5"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C146" t="b">
         <v>1</v>
@@ -2017,7 +2023,7 @@
         <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="D153" s="5"/>
     </row>
@@ -2041,7 +2047,7 @@
         <v>10</v>
       </c>
       <c r="C156" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D156" s="5"/>
     </row>
@@ -2054,7 +2060,7 @@
         <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="D158" s="5"/>
     </row>
@@ -2063,96 +2069,96 @@
         <v>7</v>
       </c>
       <c r="C159" t="s">
-        <v>12</v>
-      </c>
-      <c r="D159" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C160" s="7"/>
-      <c r="D160" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D159" s="5"/>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D160" s="5"/>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C161" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D161" s="5"/>
     </row>
-    <row r="162" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="163" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B163" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D163" s="3"/>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="4"/>
+      <c r="D162" s="5"/>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163" t="s">
+        <v>83</v>
+      </c>
+      <c r="D163" s="5"/>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C164" t="b">
-        <v>1</v>
-      </c>
-      <c r="D164" s="5"/>
-    </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C165" t="s">
-        <v>56</v>
-      </c>
-      <c r="D165" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C164" t="s">
+        <v>12</v>
+      </c>
+      <c r="D164" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B165" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C165" s="7"/>
+      <c r="D165" s="8"/>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="4" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="C166" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D166" s="5"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B167" s="4"/>
-      <c r="D167" s="5"/>
-    </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C168" t="s">
-        <v>29</v>
-      </c>
-      <c r="D168" s="5"/>
+    <row r="167" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="168" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B168" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D168" s="3"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C169" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C169" t="b">
+        <v>1</v>
       </c>
       <c r="D169" s="5"/>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C170" t="s">
+        <v>54</v>
       </c>
       <c r="D170" s="5"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C171" t="b">
         <v>1</v>
@@ -2168,7 +2174,7 @@
         <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D173" s="5"/>
     </row>
@@ -2192,7 +2198,7 @@
         <v>10</v>
       </c>
       <c r="C176" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D176" s="5"/>
     </row>
@@ -2205,7 +2211,7 @@
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="D178" s="5"/>
     </row>
@@ -2214,11 +2220,9 @@
         <v>7</v>
       </c>
       <c r="C179" t="s">
-        <v>12</v>
-      </c>
-      <c r="D179" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D179" s="5"/>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="4" t="s">
@@ -2244,7 +2248,7 @@
         <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D183" s="5"/>
     </row>
@@ -2253,9 +2257,11 @@
         <v>7</v>
       </c>
       <c r="C184" t="s">
-        <v>8</v>
-      </c>
-      <c r="D184" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D184" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
@@ -2281,7 +2287,7 @@
         <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D188" s="5"/>
     </row>
@@ -2290,18 +2296,13 @@
         <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>47</v>
-      </c>
-      <c r="D189" s="5" t="s">
-        <v>61</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D189" s="5"/>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C190" t="s">
-        <v>62</v>
       </c>
       <c r="D190" s="5"/>
     </row>
@@ -2323,7 +2324,7 @@
         <v>5</v>
       </c>
       <c r="C193" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D193" s="5"/>
     </row>
@@ -2332,16 +2333,20 @@
         <v>7</v>
       </c>
       <c r="C194" t="s">
-        <v>8</v>
-      </c>
-      <c r="D194" s="5"/>
-    </row>
-    <row r="195" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B195" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C195" s="7"/>
-      <c r="D195" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="D194" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195" t="s">
+        <v>60</v>
+      </c>
+      <c r="D195" s="5"/>
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B196" s="4" t="s">
@@ -2352,82 +2357,78 @@
       </c>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="198" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B198" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D198" s="3"/>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="4"/>
+      <c r="D197" s="5"/>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B198" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C198" t="s">
+        <v>61</v>
+      </c>
+      <c r="D198" s="5"/>
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B199" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C199" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C199" t="s">
+        <v>8</v>
       </c>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B200" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C200" t="s">
-        <v>65</v>
-      </c>
-      <c r="D200" s="5"/>
+    <row r="200" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B200" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C200" s="7"/>
+      <c r="D200" s="8"/>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="4" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="C201" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B202" s="4"/>
-      <c r="D202" s="5"/>
-    </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B203" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C203" t="s">
-        <v>66</v>
-      </c>
-      <c r="D203" s="5"/>
+    <row r="202" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="203" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D203" s="3"/>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C204" t="s">
-        <v>12</v>
-      </c>
-      <c r="D204" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C204" t="b">
+        <v>1</v>
+      </c>
+      <c r="D204" s="5"/>
     </row>
     <row r="205" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B205" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C205" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D205" s="5"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C206" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D206" s="5"/>
     </row>
@@ -2440,7 +2441,7 @@
         <v>5</v>
       </c>
       <c r="C208" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D208" s="5"/>
     </row>
@@ -2449,13 +2450,18 @@
         <v>7</v>
       </c>
       <c r="C209" t="s">
-        <v>8</v>
-      </c>
-      <c r="D209" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D209" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B210" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="C210" t="s">
+        <v>37</v>
       </c>
       <c r="D210" s="5"/>
     </row>
@@ -2477,7 +2483,7 @@
         <v>5</v>
       </c>
       <c r="C213" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D213" s="5"/>
     </row>
@@ -2490,12 +2496,11 @@
       </c>
       <c r="D214" s="5"/>
     </row>
-    <row r="215" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B215" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C215" s="7"/>
-      <c r="D215" s="8"/>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B215" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D215" s="5"/>
     </row>
     <row r="216" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B216" s="4" t="s">
@@ -2506,74 +2511,75 @@
       </c>
       <c r="D216" s="5"/>
     </row>
-    <row r="217" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="218" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B218" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D218" s="3"/>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B217" s="4"/>
+      <c r="D217" s="5"/>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B218" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C218" t="s">
+        <v>66</v>
+      </c>
+      <c r="D218" s="5"/>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B219" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C219" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C219" t="s">
+        <v>8</v>
       </c>
       <c r="D219" s="5"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B220" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C220" t="s">
-        <v>70</v>
-      </c>
-      <c r="D220" s="5"/>
+    <row r="220" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B220" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220" s="7"/>
+      <c r="D220" s="8"/>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="C221" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D221" s="5"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B222" s="4"/>
-      <c r="D222" s="5"/>
-    </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B223" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C223" t="s">
-        <v>71</v>
-      </c>
-      <c r="D223" s="5"/>
+    <row r="222" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="223" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D223" s="3"/>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C224" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C224" t="b">
+        <v>1</v>
       </c>
       <c r="D224" s="5"/>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C225" t="s">
+        <v>68</v>
       </c>
       <c r="D225" s="5"/>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C226" t="b">
         <v>1</v>
@@ -2589,7 +2595,7 @@
         <v>5</v>
       </c>
       <c r="C228" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D228" s="5"/>
     </row>
@@ -2626,7 +2632,7 @@
         <v>5</v>
       </c>
       <c r="C233" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D233" s="5"/>
     </row>
@@ -2650,7 +2656,7 @@
         <v>10</v>
       </c>
       <c r="C236" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D236" s="5"/>
     </row>
@@ -2663,7 +2669,7 @@
         <v>5</v>
       </c>
       <c r="C238" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D238" s="5"/>
     </row>
@@ -2679,9 +2685,6 @@
     <row r="240" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B240" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C240">
-        <v>1</v>
       </c>
       <c r="D240" s="5"/>
     </row>
@@ -2703,7 +2706,7 @@
         <v>5</v>
       </c>
       <c r="C243" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D243" s="5"/>
     </row>
@@ -2716,14 +2719,14 @@
       </c>
       <c r="D244" s="5"/>
     </row>
-    <row r="245" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B245" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C245" s="7">
-        <v>1</v>
-      </c>
-      <c r="D245" s="8"/>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B245" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245" s="5"/>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="4" t="s">
@@ -2734,74 +2737,77 @@
       </c>
       <c r="D246" s="5"/>
     </row>
-    <row r="247" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="248" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B248" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C248" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D248" s="3"/>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B247" s="4"/>
+      <c r="D247" s="5"/>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B248" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C248" t="s">
+        <v>73</v>
+      </c>
+      <c r="D248" s="5"/>
     </row>
     <row r="249" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B249" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C249" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C249" t="s">
+        <v>8</v>
       </c>
       <c r="D249" s="5"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B250" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C250" t="s">
-        <v>77</v>
-      </c>
-      <c r="D250" s="5"/>
+    <row r="250" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B250" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C250" s="7">
+        <v>1</v>
+      </c>
+      <c r="D250" s="8"/>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" s="4" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="C251" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D251" s="5"/>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B252" s="4"/>
-      <c r="D252" s="5"/>
-    </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B253" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C253" t="s">
-        <v>29</v>
-      </c>
-      <c r="D253" s="5"/>
+    <row r="252" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="253" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D253" s="3"/>
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B254" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C254" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C254" t="b">
+        <v>1</v>
       </c>
       <c r="D254" s="5"/>
     </row>
     <row r="255" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B255" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C255" t="s">
+        <v>75</v>
       </c>
       <c r="D255" s="5"/>
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B256" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C256" t="b">
         <v>1</v>
@@ -2817,7 +2823,7 @@
         <v>5</v>
       </c>
       <c r="C258" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="D258" s="5"/>
     </row>
@@ -2841,7 +2847,7 @@
         <v>10</v>
       </c>
       <c r="C261" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D261" s="5"/>
     </row>
@@ -2854,7 +2860,7 @@
         <v>5</v>
       </c>
       <c r="C263" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D263" s="5"/>
     </row>
@@ -2863,20 +2869,15 @@
         <v>7</v>
       </c>
       <c r="C264" t="s">
-        <v>12</v>
-      </c>
-      <c r="D264" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="265" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B265" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C265" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D265" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D264" s="5"/>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B265" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D265" s="5"/>
     </row>
     <row r="266" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B266" s="4" t="s">
@@ -2887,74 +2888,79 @@
       </c>
       <c r="D266" s="5"/>
     </row>
-    <row r="267" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="268" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B268" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D268" s="3"/>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B267" s="4"/>
+      <c r="D267" s="5"/>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B268" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C268" t="s">
+        <v>77</v>
+      </c>
+      <c r="D268" s="5"/>
     </row>
     <row r="269" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B269" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C269" t="b">
-        <v>1</v>
-      </c>
-      <c r="D269" s="5"/>
-    </row>
-    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B270" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C270" t="s">
-        <v>77</v>
-      </c>
-      <c r="D270" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C269" t="s">
+        <v>12</v>
+      </c>
+      <c r="D269" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="270" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B270" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C270" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D270" s="8"/>
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" s="4" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="C271" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D271" s="5"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B272" s="4"/>
-      <c r="D272" s="5"/>
-    </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B273" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C273" t="s">
-        <v>29</v>
-      </c>
-      <c r="D273" s="5"/>
+    <row r="272" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="273" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B273" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D273" s="3"/>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C274" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C274" t="b">
+        <v>1</v>
       </c>
       <c r="D274" s="5"/>
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C275" t="s">
+        <v>75</v>
       </c>
       <c r="D275" s="5"/>
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C276" t="b">
         <v>1</v>
@@ -2970,7 +2976,7 @@
         <v>5</v>
       </c>
       <c r="C278" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="D278" s="5"/>
     </row>
@@ -2994,7 +3000,7 @@
         <v>10</v>
       </c>
       <c r="C281" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D281" s="5"/>
     </row>
@@ -3007,7 +3013,7 @@
         <v>5</v>
       </c>
       <c r="C283" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D283" s="5"/>
     </row>
@@ -3016,20 +3022,15 @@
         <v>7</v>
       </c>
       <c r="C284" t="s">
-        <v>12</v>
-      </c>
-      <c r="D284" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="285" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B285" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C285" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D285" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D284" s="5"/>
+    </row>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B285" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D285" s="5"/>
     </row>
     <row r="286" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B286" s="4" t="s">
@@ -3040,80 +3041,122 @@
       </c>
       <c r="D286" s="5"/>
     </row>
-    <row r="287" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="288" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B288" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D288" s="3"/>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B287" s="4"/>
+      <c r="D287" s="5"/>
+    </row>
+    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B288" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C288" t="s">
+        <v>77</v>
+      </c>
+      <c r="D288" s="5"/>
     </row>
     <row r="289" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B289" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C289" t="b">
-        <v>1</v>
-      </c>
-      <c r="D289" s="5"/>
-    </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B290" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C290" t="s">
-        <v>77</v>
-      </c>
-      <c r="D290" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C289" t="s">
+        <v>12</v>
+      </c>
+      <c r="D289" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="290" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B290" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C290" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D290" s="8"/>
     </row>
     <row r="291" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B291" s="4" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="C291" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D291" s="5"/>
     </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B292" s="4"/>
-      <c r="D292" s="5"/>
-    </row>
-    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B293" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C293" t="s">
-        <v>85</v>
-      </c>
-      <c r="D293" s="5"/>
+    <row r="292" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="293" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B293" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D293" s="3"/>
     </row>
     <row r="294" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B294" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C294" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C294" t="b">
+        <v>1</v>
       </c>
       <c r="D294" s="5"/>
     </row>
-    <row r="295" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B295" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C295" s="7"/>
-      <c r="D295" s="8"/>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B295" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C295" t="s">
+        <v>75</v>
+      </c>
+      <c r="D295" s="5"/>
     </row>
     <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C296" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D296" s="5"/>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B297" s="4"/>
+      <c r="D297" s="5"/>
+    </row>
+    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B298" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C298" t="s">
+        <v>83</v>
+      </c>
+      <c r="D298" s="5"/>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B299" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C299" t="s">
+        <v>8</v>
+      </c>
+      <c r="D299" s="5"/>
+    </row>
+    <row r="300" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B300" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C300" s="7"/>
+      <c r="D300" s="8"/>
+    </row>
+    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B301" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C301" t="b">
+        <v>0</v>
+      </c>
+      <c r="D301" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjusted Step to include elution method. Low Artifact vs Proteomics
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03309A35-0BA3-4F54-9567-B9EF893E3C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0A5D3-EE0C-4526-B1F8-96E299F094C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="93">
   <si>
     <t>Step</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>100,200</t>
+  </si>
+  <si>
+    <t>Elution Method</t>
+  </si>
+  <si>
+    <t>Low Artifact</t>
+  </si>
+  <si>
+    <t>Low Artifact,Proteomics</t>
   </si>
 </sst>
 </file>
@@ -427,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -438,6 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,10 +856,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:D301"/>
+  <dimension ref="B1:D306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,74 +2138,82 @@
       </c>
       <c r="D166" s="5"/>
     </row>
-    <row r="167" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="168" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B168" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D168" s="3"/>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="10"/>
+      <c r="D167" s="10"/>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C168" t="s">
+        <v>90</v>
+      </c>
+      <c r="D168" s="5"/>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C169" t="b">
-        <v>1</v>
-      </c>
-      <c r="D169" s="5"/>
-    </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C170" t="s">
-        <v>54</v>
-      </c>
-      <c r="D170" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C169" t="s">
+        <v>12</v>
+      </c>
+      <c r="D169" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B170" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D170" s="8"/>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="4" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C171" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D171" s="5"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" s="4"/>
-      <c r="D172" s="5"/>
-    </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C173" t="s">
-        <v>29</v>
-      </c>
-      <c r="D173" s="5"/>
+    <row r="172" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="10"/>
+      <c r="D172" s="10"/>
+    </row>
+    <row r="173" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D173" s="3"/>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C174" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C174" t="b">
+        <v>1</v>
       </c>
       <c r="D174" s="5"/>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C175" t="s">
+        <v>54</v>
       </c>
       <c r="D175" s="5"/>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C176" t="b">
         <v>1</v>
@@ -2211,7 +2229,7 @@
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D178" s="5"/>
     </row>
@@ -2235,7 +2253,7 @@
         <v>10</v>
       </c>
       <c r="C181" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D181" s="5"/>
     </row>
@@ -2248,7 +2266,7 @@
         <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D183" s="5"/>
     </row>
@@ -2257,11 +2275,9 @@
         <v>7</v>
       </c>
       <c r="C184" t="s">
-        <v>12</v>
-      </c>
-      <c r="D184" s="5" t="s">
-        <v>56</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D184" s="5"/>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
@@ -2287,7 +2303,7 @@
         <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D188" s="5"/>
     </row>
@@ -2296,9 +2312,11 @@
         <v>7</v>
       </c>
       <c r="C189" t="s">
-        <v>8</v>
-      </c>
-      <c r="D189" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D189" s="5" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="4" t="s">
@@ -2324,7 +2342,7 @@
         <v>5</v>
       </c>
       <c r="C193" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D193" s="5"/>
     </row>
@@ -2333,18 +2351,13 @@
         <v>7</v>
       </c>
       <c r="C194" t="s">
-        <v>47</v>
-      </c>
-      <c r="D194" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D194" s="5"/>
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B195" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C195" t="s">
-        <v>60</v>
       </c>
       <c r="D195" s="5"/>
     </row>
@@ -2366,7 +2379,7 @@
         <v>5</v>
       </c>
       <c r="C198" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D198" s="5"/>
     </row>
@@ -2375,16 +2388,20 @@
         <v>7</v>
       </c>
       <c r="C199" t="s">
-        <v>8</v>
-      </c>
-      <c r="D199" s="5"/>
-    </row>
-    <row r="200" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B200" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C200" s="7"/>
-      <c r="D200" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B200" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C200" t="s">
+        <v>60</v>
+      </c>
+      <c r="D200" s="5"/>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B201" s="4" t="s">
@@ -2395,82 +2412,78 @@
       </c>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="203" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B203" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D203" s="3"/>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B202" s="4"/>
+      <c r="D202" s="5"/>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B203" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C203" t="s">
+        <v>61</v>
+      </c>
+      <c r="D203" s="5"/>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C204" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C204" t="s">
+        <v>8</v>
       </c>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B205" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C205" t="s">
-        <v>63</v>
-      </c>
-      <c r="D205" s="5"/>
+    <row r="205" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B205" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C205" s="7"/>
+      <c r="D205" s="8"/>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B206" s="4" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C206" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D206" s="5"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="4"/>
-      <c r="D207" s="5"/>
-    </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B208" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C208" t="s">
-        <v>64</v>
-      </c>
-      <c r="D208" s="5"/>
+    <row r="207" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="208" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B208" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D208" s="3"/>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B209" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C209" t="s">
-        <v>12</v>
-      </c>
-      <c r="D209" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C209" t="b">
+        <v>1</v>
+      </c>
+      <c r="D209" s="5"/>
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B210" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C210" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D210" s="5"/>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B211" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C211" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D211" s="5"/>
     </row>
@@ -2483,7 +2496,7 @@
         <v>5</v>
       </c>
       <c r="C213" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D213" s="5"/>
     </row>
@@ -2492,13 +2505,18 @@
         <v>7</v>
       </c>
       <c r="C214" t="s">
-        <v>8</v>
-      </c>
-      <c r="D214" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D214" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B215" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="C215" t="s">
+        <v>37</v>
       </c>
       <c r="D215" s="5"/>
     </row>
@@ -2520,7 +2538,7 @@
         <v>5</v>
       </c>
       <c r="C218" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D218" s="5"/>
     </row>
@@ -2533,12 +2551,11 @@
       </c>
       <c r="D219" s="5"/>
     </row>
-    <row r="220" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B220" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C220" s="7"/>
-      <c r="D220" s="8"/>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B220" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D220" s="5"/>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
@@ -2549,74 +2566,75 @@
       </c>
       <c r="D221" s="5"/>
     </row>
-    <row r="222" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B223" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D223" s="3"/>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B222" s="4"/>
+      <c r="D222" s="5"/>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B223" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C223" t="s">
+        <v>66</v>
+      </c>
+      <c r="D223" s="5"/>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C224" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C224" t="s">
+        <v>8</v>
       </c>
       <c r="D224" s="5"/>
     </row>
-    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B225" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C225" t="s">
-        <v>68</v>
-      </c>
-      <c r="D225" s="5"/>
+    <row r="225" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B225" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C225" s="7"/>
+      <c r="D225" s="8"/>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C226" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D226" s="5"/>
     </row>
-    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B227" s="4"/>
-      <c r="D227" s="5"/>
-    </row>
-    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B228" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C228" t="s">
-        <v>69</v>
-      </c>
-      <c r="D228" s="5"/>
+    <row r="227" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="228" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B228" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D228" s="3"/>
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B229" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C229" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C229" t="b">
+        <v>1</v>
       </c>
       <c r="D229" s="5"/>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C230" t="s">
+        <v>68</v>
       </c>
       <c r="D230" s="5"/>
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B231" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C231" t="b">
         <v>1</v>
@@ -2632,7 +2650,7 @@
         <v>5</v>
       </c>
       <c r="C233" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D233" s="5"/>
     </row>
@@ -2669,7 +2687,7 @@
         <v>5</v>
       </c>
       <c r="C238" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D238" s="5"/>
     </row>
@@ -2693,7 +2711,7 @@
         <v>10</v>
       </c>
       <c r="C241" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D241" s="5"/>
     </row>
@@ -2706,7 +2724,7 @@
         <v>5</v>
       </c>
       <c r="C243" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D243" s="5"/>
     </row>
@@ -2722,9 +2740,6 @@
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C245">
-        <v>1</v>
       </c>
       <c r="D245" s="5"/>
     </row>
@@ -2746,7 +2761,7 @@
         <v>5</v>
       </c>
       <c r="C248" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D248" s="5"/>
     </row>
@@ -2759,14 +2774,14 @@
       </c>
       <c r="D249" s="5"/>
     </row>
-    <row r="250" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B250" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C250" s="7">
-        <v>1</v>
-      </c>
-      <c r="D250" s="8"/>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B250" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250" s="5"/>
     </row>
     <row r="251" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B251" s="4" t="s">
@@ -2777,74 +2792,77 @@
       </c>
       <c r="D251" s="5"/>
     </row>
-    <row r="252" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="253" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B253" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D253" s="3"/>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252" s="4"/>
+      <c r="D252" s="5"/>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B253" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C253" t="s">
+        <v>73</v>
+      </c>
+      <c r="D253" s="5"/>
     </row>
     <row r="254" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B254" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C254" t="b">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C254" t="s">
+        <v>8</v>
       </c>
       <c r="D254" s="5"/>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B255" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C255" t="s">
-        <v>75</v>
-      </c>
-      <c r="D255" s="5"/>
+    <row r="255" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B255" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C255" s="7">
+        <v>1</v>
+      </c>
+      <c r="D255" s="8"/>
     </row>
     <row r="256" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B256" s="4" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C256" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D256" s="5"/>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B257" s="4"/>
-      <c r="D257" s="5"/>
-    </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B258" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C258" t="s">
-        <v>29</v>
-      </c>
-      <c r="D258" s="5"/>
+    <row r="257" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="258" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B258" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D258" s="3"/>
     </row>
     <row r="259" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B259" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C259" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C259" t="b">
+        <v>1</v>
       </c>
       <c r="D259" s="5"/>
     </row>
     <row r="260" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B260" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C260" t="s">
+        <v>75</v>
       </c>
       <c r="D260" s="5"/>
     </row>
     <row r="261" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B261" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C261" t="b">
         <v>1</v>
@@ -2860,7 +2878,7 @@
         <v>5</v>
       </c>
       <c r="C263" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="D263" s="5"/>
     </row>
@@ -2884,7 +2902,7 @@
         <v>10</v>
       </c>
       <c r="C266" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D266" s="5"/>
     </row>
@@ -2897,7 +2915,7 @@
         <v>5</v>
       </c>
       <c r="C268" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D268" s="5"/>
     </row>
@@ -2906,20 +2924,15 @@
         <v>7</v>
       </c>
       <c r="C269" t="s">
-        <v>12</v>
-      </c>
-      <c r="D269" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="270" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B270" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C270" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D270" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D269" s="5"/>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B270" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D270" s="5"/>
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" s="4" t="s">
@@ -2930,74 +2943,79 @@
       </c>
       <c r="D271" s="5"/>
     </row>
-    <row r="272" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="273" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B273" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C273" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D273" s="3"/>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B272" s="4"/>
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B273" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C273" t="s">
+        <v>77</v>
+      </c>
+      <c r="D273" s="5"/>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C274" t="b">
-        <v>1</v>
-      </c>
-      <c r="D274" s="5"/>
-    </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B275" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C275" t="s">
-        <v>75</v>
-      </c>
-      <c r="D275" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C274" t="s">
+        <v>12</v>
+      </c>
+      <c r="D274" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="275" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B275" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C275" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D275" s="8"/>
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="4" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C276" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D276" s="5"/>
     </row>
-    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B277" s="4"/>
-      <c r="D277" s="5"/>
-    </row>
-    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B278" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C278" t="s">
-        <v>29</v>
-      </c>
-      <c r="D278" s="5"/>
+    <row r="277" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="278" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B278" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D278" s="3"/>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B279" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C279" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C279" t="b">
+        <v>1</v>
       </c>
       <c r="D279" s="5"/>
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="C280" t="s">
+        <v>75</v>
       </c>
       <c r="D280" s="5"/>
     </row>
     <row r="281" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B281" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C281" t="b">
         <v>1</v>
@@ -3013,7 +3031,7 @@
         <v>5</v>
       </c>
       <c r="C283" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="D283" s="5"/>
     </row>
@@ -3037,7 +3055,7 @@
         <v>10</v>
       </c>
       <c r="C286" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D286" s="5"/>
     </row>
@@ -3050,7 +3068,7 @@
         <v>5</v>
       </c>
       <c r="C288" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D288" s="5"/>
     </row>
@@ -3059,20 +3077,15 @@
         <v>7</v>
       </c>
       <c r="C289" t="s">
-        <v>12</v>
-      </c>
-      <c r="D289" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="290" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B290" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C290" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D290" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D289" s="5"/>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B290" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D290" s="5"/>
     </row>
     <row r="291" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B291" s="4" t="s">
@@ -3083,80 +3096,122 @@
       </c>
       <c r="D291" s="5"/>
     </row>
-    <row r="292" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="293" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B293" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D293" s="3"/>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B292" s="4"/>
+      <c r="D292" s="5"/>
+    </row>
+    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B293" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C293" t="s">
+        <v>77</v>
+      </c>
+      <c r="D293" s="5"/>
     </row>
     <row r="294" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B294" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C294" t="b">
-        <v>1</v>
-      </c>
-      <c r="D294" s="5"/>
-    </row>
-    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B295" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C295" t="s">
-        <v>75</v>
-      </c>
-      <c r="D295" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C294" t="s">
+        <v>12</v>
+      </c>
+      <c r="D294" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="295" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B295" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C295" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D295" s="8"/>
     </row>
     <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" s="4" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="C296" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D296" s="5"/>
     </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B297" s="4"/>
-      <c r="D297" s="5"/>
-    </row>
-    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B298" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C298" t="s">
-        <v>83</v>
-      </c>
-      <c r="D298" s="5"/>
+    <row r="297" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="298" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B298" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D298" s="3"/>
     </row>
     <row r="299" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B299" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C299" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C299" t="b">
+        <v>1</v>
       </c>
       <c r="D299" s="5"/>
     </row>
-    <row r="300" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B300" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C300" s="7"/>
-      <c r="D300" s="8"/>
+    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B300" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C300" t="s">
+        <v>75</v>
+      </c>
+      <c r="D300" s="5"/>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" s="4" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="C301" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D301" s="5"/>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B302" s="4"/>
+      <c r="D302" s="5"/>
+    </row>
+    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B303" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C303" t="s">
+        <v>83</v>
+      </c>
+      <c r="D303" s="5"/>
+    </row>
+    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B304" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C304" t="s">
+        <v>8</v>
+      </c>
+      <c r="D304" s="5"/>
+    </row>
+    <row r="305" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B305" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C305" s="7"/>
+      <c r="D305" s="8"/>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B306" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C306" t="b">
+        <v>0</v>
+      </c>
+      <c r="D306" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Almost finished with desalting
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD0A5D3-EE0C-4526-B1F8-96E299F094C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B03E49-7CDE-4376-81F6-2E8EAC2001F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -303,16 +303,16 @@
     <t>IMCS SizeX Desalt</t>
   </si>
   <si>
-    <t>100,200</t>
-  </si>
-  <si>
     <t>Elution Method</t>
   </si>
   <si>
     <t>Low Artifact</t>
   </si>
   <si>
-    <t>Low Artifact,Proteomics</t>
+    <t>Low Artifact,HCP/Proteomics</t>
+  </si>
+  <si>
+    <t>100,100;100</t>
   </si>
 </sst>
 </file>
@@ -859,7 +859,7 @@
   <dimension ref="B1:D306"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,7 +2119,7 @@
         <v>12</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="165" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2147,7 +2147,7 @@
         <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D168" s="5"/>
     </row>
@@ -2159,7 +2159,7 @@
         <v>12</v>
       </c>
       <c r="D169" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="170" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2167,7 +2167,7 @@
         <v>9</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D170" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added new UV block
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B03E49-7CDE-4376-81F6-2E8EAC2001F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233B3141-850C-4403-B684-696D3126ACE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="94">
   <si>
     <t>Step</t>
   </si>
@@ -309,10 +309,13 @@
     <t>Low Artifact</t>
   </si>
   <si>
-    <t>Low Artifact,HCP/Proteomics</t>
-  </si>
-  <si>
-    <t>100,100;100</t>
+    <t>100,100 + 100</t>
+  </si>
+  <si>
+    <t>MAM/Low Artifact,HCP/Proteomics</t>
+  </si>
+  <si>
+    <t>96 Well PCR Plate,96 Well UV Plate</t>
   </si>
 </sst>
 </file>
@@ -858,8 +861,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:D306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D165" sqref="D165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +967,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2119,7 +2122,7 @@
         <v>12</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="165" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2159,7 +2162,7 @@
         <v>12</v>
       </c>
       <c r="D169" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="170" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Harmonizing Help Document and Building Blocks and method
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47017979-985E-417B-B3F4-38741F1B90F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A6420A-266D-45E8-BA28-97EAD570EA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31185" yWindow="2790" windowWidth="18900" windowHeight="11055" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="124">
   <si>
     <t>Step</t>
   </si>
@@ -87,15 +87,9 @@
     <t>Plate Choice</t>
   </si>
   <si>
-    <t>Plate Name 1</t>
-  </si>
-  <si>
     <t>New Plate 1</t>
   </si>
   <si>
-    <t>Plate Name 2</t>
-  </si>
-  <si>
     <t>New Plate 2</t>
   </si>
   <si>
@@ -270,9 +264,6 @@
     <t>Preload Liquid</t>
   </si>
   <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>Mix?</t>
   </si>
   <si>
@@ -397,6 +388,24 @@
   </si>
   <si>
     <t>BookmarkName</t>
+  </si>
+  <si>
+    <t>Pathway 1</t>
+  </si>
+  <si>
+    <t>Pathway 2</t>
+  </si>
+  <si>
+    <t>Source Plate</t>
+  </si>
+  <si>
+    <t>Load Volume</t>
+  </si>
+  <si>
+    <t>No,Dispense:10,Aspirate:10,Dispense:10;Aspirate:10</t>
+  </si>
+  <si>
+    <t>Dispense:10</t>
   </si>
 </sst>
 </file>
@@ -942,8 +951,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="B319" sqref="B319"/>
+    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
+      <selection activeCell="C322" sqref="C322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,23 +974,23 @@
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -993,10 +1002,10 @@
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -1008,40 +1017,40 @@
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -1070,10 +1079,10 @@
       </c>
       <c r="D10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1082,10 +1091,10 @@
       </c>
       <c r="D11" s="5"/>
       <c r="F11" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -1097,20 +1106,20 @@
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="F13" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1132,13 +1141,13 @@
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1150,10 +1159,10 @@
       </c>
       <c r="D16" s="8"/>
       <c r="F16" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1165,18 +1174,18 @@
       </c>
       <c r="D17" s="5"/>
       <c r="F17" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1192,17 +1201,17 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1214,10 +1223,10 @@
       </c>
       <c r="D21" s="5"/>
       <c r="F21" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -1229,30 +1238,30 @@
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -1265,10 +1274,10 @@
       <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="F25" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1280,10 +1289,10 @@
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1291,16 +1300,16 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1309,10 +1318,10 @@
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1330,10 +1339,10 @@
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1341,14 +1350,14 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="D31" s="5"/>
       <c r="F31" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1360,10 +1369,10 @@
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -1371,14 +1380,14 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D33" s="5"/>
       <c r="F33" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -1396,10 +1405,10 @@
       <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1407,14 +1416,14 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="D36" s="5"/>
       <c r="F36" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1426,10 +1435,10 @@
       </c>
       <c r="D37" s="5"/>
       <c r="F37" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1437,14 +1446,14 @@
         <v>9</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D38" s="8"/>
       <c r="F38" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1462,16 +1471,16 @@
         <v>0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D42" s="5"/>
     </row>
@@ -1489,13 +1498,13 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C45" t="b">
         <v>1</v>
@@ -1504,10 +1513,10 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D46" s="5"/>
     </row>
@@ -1520,7 +1529,7 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D48" s="5"/>
     </row>
@@ -1557,7 +1566,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D53" s="5"/>
     </row>
@@ -1569,7 +1578,7 @@
         <v>12</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1577,7 +1586,7 @@
         <v>9</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D55" s="8"/>
     </row>
@@ -1596,16 +1605,16 @@
         <v>0</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D59" s="5"/>
     </row>
@@ -1629,7 +1638,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
@@ -1638,10 +1647,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D63" s="5"/>
     </row>
@@ -1656,16 +1665,16 @@
         <v>0</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D67" s="5"/>
     </row>
@@ -1683,13 +1692,13 @@
         <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C70" t="b">
         <v>1</v>
@@ -1698,10 +1707,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D71" s="5"/>
     </row>
@@ -1714,7 +1723,7 @@
         <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D73" s="5"/>
     </row>
@@ -1751,7 +1760,7 @@
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D78" s="5"/>
     </row>
@@ -1788,7 +1797,7 @@
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D83" s="5"/>
     </row>
@@ -1797,10 +1806,10 @@
         <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1808,7 +1817,7 @@
         <v>9</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="D85" s="8"/>
     </row>
@@ -1827,16 +1836,16 @@
         <v>0</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D88" s="3"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C89" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D89" s="5"/>
     </row>
@@ -1854,13 +1863,13 @@
         <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D91" s="5"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C92" t="b">
         <v>1</v>
@@ -1869,10 +1878,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C93" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D93" s="5"/>
     </row>
@@ -1885,7 +1894,7 @@
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D95" s="5"/>
     </row>
@@ -1922,7 +1931,7 @@
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D100" s="5"/>
     </row>
@@ -1959,7 +1968,7 @@
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D105" s="5"/>
     </row>
@@ -1996,7 +2005,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D110" s="5"/>
     </row>
@@ -2033,7 +2042,7 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D115" s="5"/>
     </row>
@@ -2070,7 +2079,7 @@
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D120" s="5"/>
     </row>
@@ -2105,16 +2114,16 @@
         <v>0</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C126" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D126" s="5"/>
     </row>
@@ -2132,13 +2141,13 @@
         <v>3</v>
       </c>
       <c r="C128" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D128" s="5"/>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C129" t="b">
         <v>1</v>
@@ -2147,10 +2156,10 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C130" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D130" s="5"/>
     </row>
@@ -2163,7 +2172,7 @@
         <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D132" s="5"/>
     </row>
@@ -2172,10 +2181,10 @@
         <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2192,7 @@
         <v>9</v>
       </c>
       <c r="C134" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D134" s="5"/>
     </row>
@@ -2205,7 +2214,7 @@
         <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D137" s="5"/>
     </row>
@@ -2242,7 +2251,7 @@
         <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D142" s="5"/>
     </row>
@@ -2279,16 +2288,16 @@
         <v>0</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D147" s="3"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C148" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D148" s="5"/>
     </row>
@@ -2306,13 +2315,13 @@
         <v>3</v>
       </c>
       <c r="C150" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D150" s="5"/>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C151" t="b">
         <v>1</v>
@@ -2321,10 +2330,10 @@
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C152" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D152" s="5"/>
     </row>
@@ -2337,7 +2346,7 @@
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="D154" s="5"/>
     </row>
@@ -2374,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D159" s="5"/>
     </row>
@@ -2411,7 +2420,7 @@
         <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D164" s="5"/>
     </row>
@@ -2448,7 +2457,7 @@
         <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="D169" s="5"/>
     </row>
@@ -2460,7 +2469,7 @@
         <v>12</v>
       </c>
       <c r="D170" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="171" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2488,7 +2497,7 @@
         <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D174" s="5"/>
     </row>
@@ -2500,7 +2509,7 @@
         <v>12</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="176" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2508,7 +2517,7 @@
         <v>9</v>
       </c>
       <c r="C176" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D176" s="8"/>
     </row>
@@ -2530,16 +2539,16 @@
         <v>0</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D179" s="3"/>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C180" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D180" s="5"/>
     </row>
@@ -2557,13 +2566,13 @@
         <v>3</v>
       </c>
       <c r="C182" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D182" s="5"/>
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C183" t="b">
         <v>1</v>
@@ -2572,10 +2581,10 @@
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C184" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D184" s="5"/>
     </row>
@@ -2588,7 +2597,7 @@
         <v>5</v>
       </c>
       <c r="C186" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D186" s="5"/>
     </row>
@@ -2625,7 +2634,7 @@
         <v>5</v>
       </c>
       <c r="C191" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D191" s="5"/>
     </row>
@@ -2662,7 +2671,7 @@
         <v>5</v>
       </c>
       <c r="C196" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D196" s="5"/>
     </row>
@@ -2674,7 +2683,7 @@
         <v>12</v>
       </c>
       <c r="D197" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
@@ -2701,7 +2710,7 @@
         <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D201" s="5"/>
     </row>
@@ -2738,7 +2747,7 @@
         <v>5</v>
       </c>
       <c r="C206" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D206" s="5"/>
     </row>
@@ -2747,10 +2756,10 @@
         <v>7</v>
       </c>
       <c r="C207" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D207" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
@@ -2758,7 +2767,7 @@
         <v>9</v>
       </c>
       <c r="C208" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D208" s="5"/>
     </row>
@@ -2780,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D211" s="5"/>
     </row>
@@ -2815,16 +2824,16 @@
         <v>0</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D216" s="3"/>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B217" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C217" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D217" s="5"/>
     </row>
@@ -2842,13 +2851,13 @@
         <v>3</v>
       </c>
       <c r="C219" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D219" s="5"/>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B220" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C220" t="b">
         <v>1</v>
@@ -2857,10 +2866,10 @@
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C221" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D221" s="5"/>
     </row>
@@ -2873,7 +2882,7 @@
         <v>5</v>
       </c>
       <c r="C223" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D223" s="5"/>
     </row>
@@ -2885,7 +2894,7 @@
         <v>12</v>
       </c>
       <c r="D224" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
@@ -2893,7 +2902,7 @@
         <v>9</v>
       </c>
       <c r="C225" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D225" s="5"/>
     </row>
@@ -2915,7 +2924,7 @@
         <v>5</v>
       </c>
       <c r="C228" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D228" s="5"/>
     </row>
@@ -2952,7 +2961,7 @@
         <v>5</v>
       </c>
       <c r="C233" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D233" s="5"/>
     </row>
@@ -2987,16 +2996,16 @@
         <v>0</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D238" s="3"/>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C239" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D239" s="5"/>
     </row>
@@ -3014,13 +3023,13 @@
         <v>3</v>
       </c>
       <c r="C241" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D241" s="5"/>
     </row>
     <row r="242" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B242" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C242" t="b">
         <v>1</v>
@@ -3029,10 +3038,10 @@
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C243" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D243" s="5"/>
     </row>
@@ -3045,7 +3054,7 @@
         <v>5</v>
       </c>
       <c r="C245" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D245" s="5"/>
     </row>
@@ -3082,7 +3091,7 @@
         <v>5</v>
       </c>
       <c r="C250" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D250" s="5"/>
     </row>
@@ -3119,7 +3128,7 @@
         <v>5</v>
       </c>
       <c r="C255" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D255" s="5"/>
     </row>
@@ -3156,7 +3165,7 @@
         <v>5</v>
       </c>
       <c r="C260" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D260" s="5"/>
     </row>
@@ -3196,7 +3205,7 @@
         <v>5</v>
       </c>
       <c r="C265" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D265" s="5"/>
     </row>
@@ -3233,16 +3242,16 @@
         <v>0</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D270" s="3"/>
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C271" t="s">
         <v>89</v>
-      </c>
-      <c r="C271" t="s">
-        <v>92</v>
       </c>
       <c r="D271" s="5"/>
     </row>
@@ -3260,13 +3269,13 @@
         <v>3</v>
       </c>
       <c r="C273" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D273" s="5"/>
     </row>
     <row r="274" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B274" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C274" t="b">
         <v>1</v>
@@ -3275,10 +3284,10 @@
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C275" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D275" s="5"/>
     </row>
@@ -3291,7 +3300,7 @@
         <v>5</v>
       </c>
       <c r="C277" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D277" s="5"/>
     </row>
@@ -3328,7 +3337,7 @@
         <v>5</v>
       </c>
       <c r="C282" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D282" s="5"/>
     </row>
@@ -3365,7 +3374,7 @@
         <v>5</v>
       </c>
       <c r="C287" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D287" s="5"/>
     </row>
@@ -3377,7 +3386,7 @@
         <v>12</v>
       </c>
       <c r="D288" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="289" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3385,7 +3394,7 @@
         <v>9</v>
       </c>
       <c r="C289" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D289" s="8"/>
     </row>
@@ -3404,16 +3413,16 @@
         <v>0</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D292" s="3"/>
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C293" t="s">
         <v>89</v>
-      </c>
-      <c r="C293" t="s">
-        <v>92</v>
       </c>
       <c r="D293" s="5"/>
     </row>
@@ -3431,13 +3440,13 @@
         <v>3</v>
       </c>
       <c r="C295" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D295" s="5"/>
     </row>
     <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C296" t="b">
         <v>1</v>
@@ -3446,10 +3455,10 @@
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C297" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D297" s="5"/>
     </row>
@@ -3462,7 +3471,7 @@
         <v>5</v>
       </c>
       <c r="C299" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D299" s="5"/>
     </row>
@@ -3499,7 +3508,7 @@
         <v>5</v>
       </c>
       <c r="C304" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D304" s="5"/>
     </row>
@@ -3536,7 +3545,7 @@
         <v>5</v>
       </c>
       <c r="C309" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D309" s="5"/>
     </row>
@@ -3548,7 +3557,7 @@
         <v>12</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="311" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3556,7 +3565,7 @@
         <v>9</v>
       </c>
       <c r="C311" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D311" s="8"/>
     </row>
@@ -3575,16 +3584,16 @@
         <v>0</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D314" s="3"/>
     </row>
     <row r="315" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B315" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C315" t="s">
         <v>89</v>
-      </c>
-      <c r="C315" t="s">
-        <v>92</v>
       </c>
       <c r="D315" s="5"/>
     </row>
@@ -3602,13 +3611,13 @@
         <v>3</v>
       </c>
       <c r="C317" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D317" s="5"/>
     </row>
     <row r="318" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B318" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C318" t="b">
         <v>1</v>
@@ -3617,10 +3626,10 @@
     </row>
     <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C319" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D319" s="5"/>
     </row>
@@ -3633,7 +3642,7 @@
         <v>5</v>
       </c>
       <c r="C321" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="D321" s="5"/>
     </row>

</xml_diff>

<commit_message>
Connected the method editor to the Word Help Document
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A6420A-266D-45E8-BA28-97EAD570EA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66255EBF-30A8-4220-9D11-9031869C9736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="138">
   <si>
     <t>Step</t>
   </si>
@@ -303,9 +303,6 @@
     <t>Actions</t>
   </si>
   <si>
-    <t>Modifiers (Advanced)</t>
-  </si>
-  <si>
     <t>Solutions</t>
   </si>
   <si>
@@ -406,6 +403,51 @@
   </si>
   <si>
     <t>Dispense:10</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsPlate</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsSplitPlate</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsMergePlates</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsFinish</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsLiquidTransfer</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsDilute</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsIncubate</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsIMCSSizeXDesalt</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsVacuum</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsNotify</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsMagneticBeads</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsAliquot</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsPool</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsPreloadLiquid</t>
+  </si>
+  <si>
+    <t>Modifiers</t>
   </si>
 </sst>
 </file>
@@ -951,8 +993,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A302" workbookViewId="0">
-      <selection activeCell="C322" sqref="C322"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="C316" sqref="C316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,7 +1016,7 @@
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -987,10 +1029,10 @@
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1002,7 +1044,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>28</v>
@@ -1017,10 +1059,10 @@
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1032,25 +1074,25 @@
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="D7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -1079,10 +1121,10 @@
       </c>
       <c r="D10" s="5"/>
       <c r="F10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1091,10 +1133,10 @@
       </c>
       <c r="D11" s="5"/>
       <c r="F11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -1106,20 +1148,20 @@
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="F13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1144,10 +1186,10 @@
         <v>84</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1159,10 +1201,10 @@
       </c>
       <c r="D16" s="8"/>
       <c r="F16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1174,18 +1216,18 @@
       </c>
       <c r="D17" s="5"/>
       <c r="F17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1208,10 +1250,10 @@
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1223,10 +1265,10 @@
       </c>
       <c r="D21" s="5"/>
       <c r="F21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -1238,10 +1280,10 @@
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1253,18 +1295,18 @@
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="4"/>
@@ -1274,10 +1316,10 @@
       <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="F25" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1289,10 +1331,10 @@
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1303,13 +1345,13 @@
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1318,10 +1360,10 @@
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1339,10 +1381,10 @@
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1350,14 +1392,14 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D31" s="5"/>
       <c r="F31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1369,10 +1411,10 @@
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -1384,10 +1426,10 @@
       </c>
       <c r="D33" s="5"/>
       <c r="F33" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -1405,10 +1447,10 @@
       <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1416,14 +1458,14 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D36" s="5"/>
       <c r="F36" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1435,10 +1477,10 @@
       </c>
       <c r="D37" s="5"/>
       <c r="F37" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1450,10 +1492,10 @@
       </c>
       <c r="D38" s="8"/>
       <c r="F38" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1513,10 +1555,10 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="D46" s="5"/>
     </row>
@@ -1647,10 +1689,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="D63" s="5"/>
     </row>
@@ -1707,10 +1749,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C71" t="s">
-        <v>25</v>
+        <v>127</v>
       </c>
       <c r="D71" s="5"/>
     </row>
@@ -1809,7 +1851,7 @@
         <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1817,7 +1859,7 @@
         <v>9</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D85" s="8"/>
     </row>
@@ -1878,10 +1920,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C93" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="D93" s="5"/>
     </row>
@@ -2156,10 +2198,10 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C130" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D130" s="5"/>
     </row>
@@ -2330,10 +2372,10 @@
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C152" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="D152" s="5"/>
     </row>
@@ -2346,7 +2388,7 @@
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D154" s="5"/>
     </row>
@@ -2457,7 +2499,7 @@
         <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D169" s="5"/>
     </row>
@@ -2581,10 +2623,10 @@
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C184" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="D184" s="5"/>
     </row>
@@ -2866,10 +2908,10 @@
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C221" t="s">
-        <v>56</v>
+        <v>132</v>
       </c>
       <c r="D221" s="5"/>
     </row>
@@ -3038,10 +3080,10 @@
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C243" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="D243" s="5"/>
     </row>
@@ -3205,7 +3247,7 @@
         <v>5</v>
       </c>
       <c r="C265" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D265" s="5"/>
     </row>
@@ -3251,7 +3293,7 @@
         <v>86</v>
       </c>
       <c r="C271" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="D271" s="5"/>
     </row>
@@ -3284,10 +3326,10 @@
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C275" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="D275" s="5"/>
     </row>
@@ -3422,7 +3464,7 @@
         <v>86</v>
       </c>
       <c r="C293" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="D293" s="5"/>
     </row>
@@ -3455,10 +3497,10 @@
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C297" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="D297" s="5"/>
     </row>
@@ -3593,7 +3635,7 @@
         <v>86</v>
       </c>
       <c r="C315" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="D315" s="5"/>
     </row>
@@ -3626,10 +3668,10 @@
     </row>
     <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C319" t="s">
-        <v>75</v>
+        <v>136</v>
       </c>
       <c r="D319" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added Plate as solution category. Forgot it.
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66255EBF-30A8-4220-9D11-9031869C9736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B99C8B5-8E34-42BD-B95B-58ED17469A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
+    <sheet name="Colors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="139">
   <si>
     <t>Step</t>
   </si>
@@ -309,9 +310,6 @@
     <t>Categories</t>
   </si>
   <si>
-    <t>General Reagent,Reductant,Alkylant,Quench,Buffer/Diluent,Denaturant,Enzyme</t>
-  </si>
-  <si>
     <t>Storage Temperatures</t>
   </si>
   <si>
@@ -448,6 +446,12 @@
   </si>
   <si>
     <t>Modifiers</t>
+  </si>
+  <si>
+    <t>General Reagent,Reductant,Alkylant,Quench,Buffer/Diluent,Denaturant,Enzyme,Plate</t>
+  </si>
+  <si>
+    <t>ECEAE4</t>
   </si>
 </sst>
 </file>
@@ -571,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -583,6 +587,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,23 +610,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>275609</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>132636</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47009</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>189786</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087DD2D1-9917-46AE-B22D-1C69CBE090DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E92CFE-7DE1-496B-A04F-72766E21AE04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -636,7 +642,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16506825" y="180975"/>
+          <a:off x="1828800" y="762000"/>
           <a:ext cx="4923809" cy="5714286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -648,23 +654,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>523276</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>66114</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>361351</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142314</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4FA910F-32CB-4367-A911-4C0E84F583EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D708502C-F841-41C4-9DD7-9DA7291364AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -680,7 +686,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15420975" y="200025"/>
+          <a:off x="7153275" y="1181100"/>
           <a:ext cx="4790476" cy="4485714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -993,8 +999,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="C316" sqref="C316"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="C318" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1038,7 @@
         <v>90</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1044,7 +1050,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>28</v>
@@ -1059,10 +1065,10 @@
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1074,25 +1080,25 @@
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -1121,10 +1127,10 @@
       </c>
       <c r="D10" s="5"/>
       <c r="F10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1133,10 +1139,10 @@
       </c>
       <c r="D11" s="5"/>
       <c r="F11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -1148,20 +1154,20 @@
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="F13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1186,10 +1192,10 @@
         <v>84</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1201,10 +1207,10 @@
       </c>
       <c r="D16" s="8"/>
       <c r="F16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1216,18 +1222,18 @@
       </c>
       <c r="D17" s="5"/>
       <c r="F17" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1250,10 +1256,10 @@
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1265,10 +1271,10 @@
       </c>
       <c r="D21" s="5"/>
       <c r="F21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -1280,10 +1286,10 @@
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1295,18 +1301,18 @@
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="4"/>
@@ -1316,10 +1322,10 @@
       <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="F25" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1331,10 +1337,10 @@
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1345,13 +1351,13 @@
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -1360,10 +1366,10 @@
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1381,10 +1387,10 @@
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1392,14 +1398,14 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D31" s="5"/>
       <c r="F31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1411,10 +1417,10 @@
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -1426,10 +1432,10 @@
       </c>
       <c r="D33" s="5"/>
       <c r="F33" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -1447,10 +1453,10 @@
       <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1458,14 +1464,14 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="5"/>
       <c r="F36" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1477,10 +1483,10 @@
       </c>
       <c r="D37" s="5"/>
       <c r="F37" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1492,10 +1498,10 @@
       </c>
       <c r="D38" s="8"/>
       <c r="F38" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1555,10 +1561,10 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D46" s="5"/>
     </row>
@@ -1689,10 +1695,10 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D63" s="5"/>
     </row>
@@ -1749,10 +1755,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C71" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D71" s="5"/>
     </row>
@@ -1851,7 +1857,7 @@
         <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1859,7 +1865,7 @@
         <v>9</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D85" s="8"/>
     </row>
@@ -1920,10 +1926,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C93" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D93" s="5"/>
     </row>
@@ -2198,10 +2204,10 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D130" s="5"/>
     </row>
@@ -2372,10 +2378,10 @@
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C152" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D152" s="5"/>
     </row>
@@ -2388,7 +2394,7 @@
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D154" s="5"/>
     </row>
@@ -2499,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D169" s="5"/>
     </row>
@@ -2623,10 +2629,10 @@
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C184" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D184" s="5"/>
     </row>
@@ -2908,10 +2914,10 @@
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C221" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D221" s="5"/>
     </row>
@@ -3080,10 +3086,10 @@
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C243" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D243" s="5"/>
     </row>
@@ -3247,7 +3253,7 @@
         <v>5</v>
       </c>
       <c r="C265" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D265" s="5"/>
     </row>
@@ -3293,7 +3299,7 @@
         <v>86</v>
       </c>
       <c r="C271" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D271" s="5"/>
     </row>
@@ -3326,10 +3332,10 @@
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C275" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D275" s="5"/>
     </row>
@@ -3464,7 +3470,7 @@
         <v>86</v>
       </c>
       <c r="C293" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D293" s="5"/>
     </row>
@@ -3497,10 +3503,10 @@
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C297" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D297" s="5"/>
     </row>
@@ -3634,8 +3640,8 @@
       <c r="B315" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C315" t="s">
-        <v>137</v>
+      <c r="C315" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="D315" s="5"/>
     </row>
@@ -3652,8 +3658,8 @@
       <c r="B317" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C317" t="s">
-        <v>68</v>
+      <c r="C317" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="D317" s="5"/>
     </row>
@@ -3668,10 +3674,10 @@
     </row>
     <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C319" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D319" s="5"/>
     </row>
@@ -3714,6 +3720,20 @@
       <c r="D324" s="5"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0353A2-A6AC-4E44-A6E3-EA2FDBE0647A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed Plate option. Lumped in with General Reagent instead
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B99C8B5-8E34-42BD-B95B-58ED17469A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109CFE1C-4989-44EF-BAEC-C6588487FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -448,10 +448,10 @@
     <t>Modifiers</t>
   </si>
   <si>
-    <t>General Reagent,Reductant,Alkylant,Quench,Buffer/Diluent,Denaturant,Enzyme,Plate</t>
-  </si>
-  <si>
     <t>ECEAE4</t>
+  </si>
+  <si>
+    <t>General Reagent/Plate,Reductant,Alkylant,Quench,Buffer/Diluent,Denaturant,Enzyme</t>
   </si>
 </sst>
 </file>
@@ -999,8 +999,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="C318" sqref="C318"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1038,7 @@
         <v>90</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -3659,7 +3659,7 @@
         <v>3</v>
       </c>
       <c r="C317" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D317" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added LLD as a solution option for cases like Chloroform that does not conduct electricity
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109CFE1C-4989-44EF-BAEC-C6588487FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BFFD84-453E-483A-8EEA-7E95962A12C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="144">
   <si>
     <t>Step</t>
   </si>
@@ -337,9 +337,6 @@
     <t>Homogenous</t>
   </si>
   <si>
-    <t>ACN/MeOH/CCL3</t>
-  </si>
-  <si>
     <t>Very High</t>
   </si>
   <si>
@@ -452,6 +449,24 @@
   </si>
   <si>
     <t>General Reagent/Plate,Reductant,Alkylant,Quench,Buffer/Diluent,Denaturant,Enzyme</t>
+  </si>
+  <si>
+    <t>Liquid Level Detection Options</t>
+  </si>
+  <si>
+    <t>Normal,Organic</t>
+  </si>
+  <si>
+    <t>Liquid Level Detection</t>
+  </si>
+  <si>
+    <t>ACN/MeOH</t>
+  </si>
+  <si>
+    <t>Chloroform</t>
+  </si>
+  <si>
+    <t>Organic</t>
   </si>
 </sst>
 </file>
@@ -999,8 +1014,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1023,7 @@
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="74.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1038,7 +1053,7 @@
         <v>90</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1065,10 +1080,10 @@
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1080,32 +1095,36 @@
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="D8" s="5"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
@@ -1178,8 +1197,12 @@
         <v>11</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
@@ -1191,12 +1214,8 @@
       <c r="D15" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="6" t="s">
@@ -1207,10 +1226,10 @@
       </c>
       <c r="D16" s="8"/>
       <c r="F16" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1222,18 +1241,18 @@
       </c>
       <c r="D17" s="5"/>
       <c r="F17" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1244,8 +1263,12 @@
         <v>14</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
@@ -1256,10 +1279,10 @@
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1270,12 +1293,8 @@
         <v>0</v>
       </c>
       <c r="D21" s="5"/>
-      <c r="F21" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
@@ -1286,10 +1305,10 @@
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1301,31 +1320,35 @@
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" s="5"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
+      <c r="F24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="F25" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1337,10 +1360,10 @@
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="4" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1351,14 +1374,10 @@
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>104</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
@@ -1366,10 +1385,10 @@
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="4" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1380,17 +1399,21 @@
         <v>0</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="5"/>
+      <c r="F29" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1398,14 +1421,14 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D31" s="5"/>
       <c r="F31" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1417,10 +1440,10 @@
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="4" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -1431,12 +1454,8 @@
         <v>17</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="F33" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>106</v>
-      </c>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
@@ -1446,17 +1465,21 @@
         <v>0</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="5"/>
+      <c r="F34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1464,14 +1487,14 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D36" s="5"/>
       <c r="F36" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1483,10 +1506,10 @@
       </c>
       <c r="D37" s="5"/>
       <c r="F37" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1497,11 +1520,11 @@
         <v>18</v>
       </c>
       <c r="D38" s="8"/>
-      <c r="F38" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>106</v>
+      <c r="F38" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -1512,8 +1535,17 @@
         <v>0</v>
       </c>
       <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F40" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="41" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
         <v>0</v>
@@ -1522,6 +1554,12 @@
         <v>19</v>
       </c>
       <c r="D41" s="3"/>
+      <c r="F41" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
@@ -1531,6 +1569,12 @@
         <v>87</v>
       </c>
       <c r="D42" s="5"/>
+      <c r="F42" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
@@ -1540,6 +1584,12 @@
         <v>0</v>
       </c>
       <c r="D43" s="5"/>
+      <c r="F43" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
@@ -1549,6 +1599,12 @@
         <v>20</v>
       </c>
       <c r="D44" s="5"/>
+      <c r="F44" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
@@ -1558,19 +1614,33 @@
         <v>1</v>
       </c>
       <c r="D45" s="5"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="5"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D46" s="5"/>
+      <c r="F46" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="D47" s="5"/>
+      <c r="F47" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
@@ -1580,8 +1650,14 @@
         <v>21</v>
       </c>
       <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F48" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="4" t="s">
         <v>7</v>
       </c>
@@ -1589,14 +1665,26 @@
         <v>8</v>
       </c>
       <c r="D49" s="5"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F49" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="5"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F50" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>10</v>
       </c>
@@ -1605,11 +1693,11 @@
       </c>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="D52" s="5"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>5</v>
       </c>
@@ -1618,7 +1706,7 @@
       </c>
       <c r="D53" s="5"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>7</v>
       </c>
@@ -1629,7 +1717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="6" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1726,7 @@
       </c>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
         <v>10</v>
       </c>
@@ -1647,8 +1735,8 @@
       </c>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B58" s="1" t="s">
         <v>0</v>
       </c>
@@ -1657,7 +1745,7 @@
       </c>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
         <v>86</v>
       </c>
@@ -1666,7 +1754,7 @@
       </c>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
         <v>2</v>
       </c>
@@ -1675,7 +1763,7 @@
       </c>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>3</v>
       </c>
@@ -1684,7 +1772,7 @@
       </c>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>78</v>
       </c>
@@ -1693,16 +1781,16 @@
       </c>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="6"/>
       <c r="C64" s="7"/>
       <c r="D64" s="8"/>
@@ -1755,10 +1843,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D71" s="5"/>
     </row>
@@ -1857,7 +1945,7 @@
         <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1865,7 +1953,7 @@
         <v>9</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D85" s="8"/>
     </row>
@@ -1926,10 +2014,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C93" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D93" s="5"/>
     </row>
@@ -2204,10 +2292,10 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D130" s="5"/>
     </row>
@@ -2378,10 +2466,10 @@
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C152" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D152" s="5"/>
     </row>
@@ -2394,7 +2482,7 @@
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D154" s="5"/>
     </row>
@@ -2505,7 +2593,7 @@
         <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D169" s="5"/>
     </row>
@@ -2629,10 +2717,10 @@
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C184" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D184" s="5"/>
     </row>
@@ -2914,10 +3002,10 @@
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B221" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C221" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D221" s="5"/>
     </row>
@@ -3086,10 +3174,10 @@
     </row>
     <row r="243" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B243" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C243" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D243" s="5"/>
     </row>
@@ -3253,7 +3341,7 @@
         <v>5</v>
       </c>
       <c r="C265" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D265" s="5"/>
     </row>
@@ -3299,7 +3387,7 @@
         <v>86</v>
       </c>
       <c r="C271" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D271" s="5"/>
     </row>
@@ -3332,10 +3420,10 @@
     </row>
     <row r="275" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B275" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C275" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D275" s="5"/>
     </row>
@@ -3470,7 +3558,7 @@
         <v>86</v>
       </c>
       <c r="C293" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D293" s="5"/>
     </row>
@@ -3503,10 +3591,10 @@
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C297" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D297" s="5"/>
     </row>
@@ -3659,7 +3747,7 @@
         <v>3</v>
       </c>
       <c r="C317" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D317" s="5"/>
     </row>
@@ -3674,10 +3762,10 @@
     </row>
     <row r="319" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B319" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C319" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D319" s="5"/>
     </row>

</xml_diff>

<commit_message>
Added wait for temperature option to Incubation Step. It is awesome!
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BFFD84-453E-483A-8EEA-7E95962A12C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BCEBF1-1EEE-4AF9-B0BA-A6695F65D705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="146">
   <si>
     <t>Step</t>
   </si>
@@ -467,6 +467,12 @@
   </si>
   <si>
     <t>Organic</t>
+  </si>
+  <si>
+    <t>Wait For Temperature?</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1018,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:G324"/>
+  <dimension ref="B1:G329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,53 +2351,58 @@
       <c r="B136" s="4"/>
       <c r="D136" s="5"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C137" t="s">
-        <v>43</v>
+      <c r="C137" s="12" t="s">
+        <v>144</v>
       </c>
       <c r="D137" s="5"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C138" t="s">
-        <v>8</v>
-      </c>
-      <c r="D138" s="5"/>
-    </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C138" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B139" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C139" s="12" t="s">
+        <v>145</v>
+      </c>
       <c r="D139" s="5"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B140" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C140" t="b">
+      <c r="C140" s="12" t="b">
         <v>0</v>
       </c>
       <c r="D140" s="5"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B141" s="4"/>
       <c r="D141" s="5"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B142" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C142" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D142" s="5"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B143" s="4" t="s">
         <v>7</v>
       </c>
@@ -2400,16 +2411,14 @@
       </c>
       <c r="D143" s="5"/>
     </row>
-    <row r="144" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C144" s="7">
-        <v>0</v>
-      </c>
-      <c r="D144" s="8"/>
-    </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C144"/>
+      <c r="D144" s="5"/>
+    </row>
+    <row r="145" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B145" s="4" t="s">
         <v>10</v>
       </c>
@@ -2418,95 +2427,98 @@
       </c>
       <c r="D145" s="5"/>
     </row>
-    <row r="146" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="147" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B147" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D147" s="3"/>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="4"/>
+      <c r="D146" s="5"/>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C147" t="s">
+        <v>44</v>
+      </c>
+      <c r="D147" s="5"/>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" s="4" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C148" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="D148" s="5"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C149" t="b">
-        <v>1</v>
-      </c>
-      <c r="D149" s="5"/>
+    <row r="149" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" s="7">
+        <v>0</v>
+      </c>
+      <c r="D149" s="8"/>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C150" t="s">
-        <v>45</v>
+        <v>10</v>
+      </c>
+      <c r="C150" t="b">
+        <v>0</v>
       </c>
       <c r="D150" s="5"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C151" t="b">
-        <v>1</v>
-      </c>
-      <c r="D151" s="5"/>
-    </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C152" t="s">
-        <v>128</v>
-      </c>
-      <c r="D152" s="5"/>
+    <row r="151" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="152" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B152" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D152" s="3"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="4"/>
+      <c r="B153" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C153" t="s">
+        <v>88</v>
+      </c>
       <c r="D153" s="5"/>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B154" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C154" t="s">
-        <v>117</v>
+        <v>2</v>
+      </c>
+      <c r="C154" t="b">
+        <v>1</v>
       </c>
       <c r="D154" s="5"/>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C155" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D155" s="5"/>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="4" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="C156" t="b">
+        <v>1</v>
       </c>
       <c r="D156" s="5"/>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C157" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="C157" t="s">
+        <v>128</v>
       </c>
       <c r="D157" s="5"/>
     </row>
@@ -2519,7 +2531,7 @@
         <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="D159" s="5"/>
     </row>
@@ -2543,7 +2555,7 @@
         <v>10</v>
       </c>
       <c r="C162" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D162" s="5"/>
     </row>
@@ -2556,7 +2568,7 @@
         <v>5</v>
       </c>
       <c r="C164" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="D164" s="5"/>
     </row>
@@ -2580,7 +2592,7 @@
         <v>10</v>
       </c>
       <c r="C167" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D167" s="5"/>
     </row>
@@ -2593,7 +2605,7 @@
         <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>118</v>
+        <v>46</v>
       </c>
       <c r="D169" s="5"/>
     </row>
@@ -2602,38 +2614,35 @@
         <v>7</v>
       </c>
       <c r="C170" t="s">
-        <v>12</v>
-      </c>
-      <c r="D170" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C171" s="7"/>
-      <c r="D171" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D170" s="5"/>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D171" s="5"/>
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C172" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D172" s="5"/>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B173" s="10"/>
-      <c r="D173" s="10"/>
+      <c r="B173" s="4"/>
+      <c r="D173" s="5"/>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="D174" s="5"/>
     </row>
@@ -2645,16 +2654,14 @@
         <v>12</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="176" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B176" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C176" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="C176" s="7"/>
       <c r="D176" s="8"/>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
@@ -2666,98 +2673,103 @@
       </c>
       <c r="D177" s="5"/>
     </row>
-    <row r="178" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" s="10"/>
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B179" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D179" s="3"/>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C179" t="s">
+        <v>81</v>
+      </c>
+      <c r="D179" s="5"/>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="4" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C180" t="s">
-        <v>88</v>
-      </c>
-      <c r="D180" s="5"/>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C181" t="b">
-        <v>1</v>
-      </c>
-      <c r="D181" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D180" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B181" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D181" s="8"/>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C182" t="s">
-        <v>48</v>
+        <v>10</v>
+      </c>
+      <c r="C182" t="b">
+        <v>0</v>
       </c>
       <c r="D182" s="5"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B183" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C183" t="b">
-        <v>1</v>
-      </c>
-      <c r="D183" s="5"/>
-    </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C184" t="s">
-        <v>129</v>
-      </c>
-      <c r="D184" s="5"/>
+    <row r="183" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" s="10"/>
+      <c r="D183" s="10"/>
+    </row>
+    <row r="184" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B184" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D184" s="3"/>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B185" s="4"/>
+      <c r="B185" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C185" t="s">
+        <v>88</v>
+      </c>
       <c r="D185" s="5"/>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C186" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="C186" t="b">
+        <v>1</v>
       </c>
       <c r="D186" s="5"/>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C187" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D187" s="5"/>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="4" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="C188" t="b">
+        <v>1</v>
       </c>
       <c r="D188" s="5"/>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C189" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="C189" t="s">
+        <v>129</v>
       </c>
       <c r="D189" s="5"/>
     </row>
@@ -2770,7 +2782,7 @@
         <v>5</v>
       </c>
       <c r="C191" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D191" s="5"/>
     </row>
@@ -2794,7 +2806,7 @@
         <v>10</v>
       </c>
       <c r="C194" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D194" s="5"/>
     </row>
@@ -2807,7 +2819,7 @@
         <v>5</v>
       </c>
       <c r="C196" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D196" s="5"/>
     </row>
@@ -2816,11 +2828,9 @@
         <v>7</v>
       </c>
       <c r="C197" t="s">
-        <v>12</v>
-      </c>
-      <c r="D197" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D197" s="5"/>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" s="4" t="s">
@@ -2846,7 +2856,7 @@
         <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D201" s="5"/>
     </row>
@@ -2855,9 +2865,11 @@
         <v>7</v>
       </c>
       <c r="C202" t="s">
-        <v>8</v>
-      </c>
-      <c r="D202" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" s="4" t="s">
@@ -2883,7 +2895,7 @@
         <v>5</v>
       </c>
       <c r="C206" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D206" s="5"/>
     </row>
@@ -2892,18 +2904,13 @@
         <v>7</v>
       </c>
       <c r="C207" t="s">
-        <v>41</v>
-      </c>
-      <c r="D207" s="5" t="s">
-        <v>53</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D207" s="5"/>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B208" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C208" t="s">
-        <v>54</v>
       </c>
       <c r="D208" s="5"/>
     </row>
@@ -2925,7 +2932,7 @@
         <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D211" s="5"/>
     </row>
@@ -2934,16 +2941,20 @@
         <v>7</v>
       </c>
       <c r="C212" t="s">
-        <v>8</v>
-      </c>
-      <c r="D212" s="5"/>
-    </row>
-    <row r="213" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B213" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C213" s="7"/>
-      <c r="D213" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="D212" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B213" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C213" t="s">
+        <v>54</v>
+      </c>
+      <c r="D213" s="5"/>
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B214" s="4" t="s">
@@ -2954,100 +2965,96 @@
       </c>
       <c r="D214" s="5"/>
     </row>
-    <row r="215" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B216" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D216" s="3"/>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B215" s="4"/>
+      <c r="D215" s="5"/>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B216" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C216" t="s">
+        <v>55</v>
+      </c>
+      <c r="D216" s="5"/>
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B217" s="4" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C217" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="D217" s="5"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B218" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C218" t="b">
-        <v>1</v>
-      </c>
-      <c r="D218" s="5"/>
+    <row r="218" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B218" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C218" s="7"/>
+      <c r="D218" s="8"/>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B219" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C219" t="s">
-        <v>57</v>
+        <v>10</v>
+      </c>
+      <c r="C219" t="b">
+        <v>0</v>
       </c>
       <c r="D219" s="5"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B220" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C220" t="b">
-        <v>1</v>
-      </c>
-      <c r="D220" s="5"/>
-    </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B221" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C221" t="s">
-        <v>130</v>
-      </c>
-      <c r="D221" s="5"/>
+    <row r="220" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="221" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D221" s="3"/>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B222" s="4"/>
+      <c r="B222" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C222" t="s">
+        <v>88</v>
+      </c>
       <c r="D222" s="5"/>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B223" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C223" t="s">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="C223" t="b">
+        <v>1</v>
       </c>
       <c r="D223" s="5"/>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B224" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C224" t="s">
-        <v>12</v>
-      </c>
-      <c r="D224" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="D224" s="5"/>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C225" t="s">
-        <v>31</v>
+        <v>78</v>
+      </c>
+      <c r="C225" t="b">
+        <v>1</v>
       </c>
       <c r="D225" s="5"/>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C226" t="b">
-        <v>0</v>
+        <v>114</v>
+      </c>
+      <c r="C226" t="s">
+        <v>130</v>
       </c>
       <c r="D226" s="5"/>
     </row>
@@ -3060,7 +3067,7 @@
         <v>5</v>
       </c>
       <c r="C228" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D228" s="5"/>
     </row>
@@ -3069,13 +3076,18 @@
         <v>7</v>
       </c>
       <c r="C229" t="s">
-        <v>8</v>
-      </c>
-      <c r="D229" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D229" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B230" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="C230" t="s">
+        <v>31</v>
       </c>
       <c r="D230" s="5"/>
     </row>
@@ -3097,7 +3109,7 @@
         <v>5</v>
       </c>
       <c r="C233" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D233" s="5"/>
     </row>
@@ -3110,12 +3122,11 @@
       </c>
       <c r="D234" s="5"/>
     </row>
-    <row r="235" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B235" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C235" s="7"/>
-      <c r="D235" s="8"/>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B235" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D235" s="5"/>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B236" s="4" t="s">
@@ -3126,95 +3137,96 @@
       </c>
       <c r="D236" s="5"/>
     </row>
-    <row r="237" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="238" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B238" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D238" s="3"/>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B237" s="4"/>
+      <c r="D237" s="5"/>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B238" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C238" t="s">
+        <v>60</v>
+      </c>
+      <c r="D238" s="5"/>
     </row>
     <row r="239" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B239" s="4" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C239" t="s">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="D239" s="5"/>
     </row>
-    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B240" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C240" t="b">
-        <v>1</v>
-      </c>
-      <c r="D240" s="5"/>
+    <row r="240" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B240" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C240" s="7"/>
+      <c r="D240" s="8"/>
     </row>
     <row r="241" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B241" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C241" t="s">
-        <v>62</v>
+        <v>10</v>
+      </c>
+      <c r="C241" t="b">
+        <v>0</v>
       </c>
       <c r="D241" s="5"/>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B242" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C242" t="b">
-        <v>1</v>
-      </c>
-      <c r="D242" s="5"/>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B243" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C243" t="s">
-        <v>131</v>
-      </c>
-      <c r="D243" s="5"/>
+    <row r="242" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="243" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D243" s="3"/>
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B244" s="4"/>
+      <c r="B244" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C244" t="s">
+        <v>88</v>
+      </c>
       <c r="D244" s="5"/>
     </row>
     <row r="245" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B245" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C245" t="s">
-        <v>63</v>
+        <v>2</v>
+      </c>
+      <c r="C245" t="b">
+        <v>1</v>
       </c>
       <c r="D245" s="5"/>
     </row>
     <row r="246" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B246" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C246" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D246" s="5"/>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="4" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="C247" t="b">
+        <v>1</v>
       </c>
       <c r="D247" s="5"/>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C248" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="C248" t="s">
+        <v>131</v>
       </c>
       <c r="D248" s="5"/>
     </row>
@@ -3227,7 +3239,7 @@
         <v>5</v>
       </c>
       <c r="C250" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D250" s="5"/>
     </row>
@@ -3264,7 +3276,7 @@
         <v>5</v>
       </c>
       <c r="C255" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D255" s="5"/>
     </row>
@@ -3288,7 +3300,7 @@
         <v>10</v>
       </c>
       <c r="C258" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D258" s="5"/>
     </row>
@@ -3301,7 +3313,7 @@
         <v>5</v>
       </c>
       <c r="C260" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D260" s="5"/>
     </row>
@@ -3317,9 +3329,6 @@
     <row r="262" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B262" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C262">
-        <v>1</v>
       </c>
       <c r="D262" s="5"/>
     </row>
@@ -3341,7 +3350,7 @@
         <v>5</v>
       </c>
       <c r="C265" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="D265" s="5"/>
     </row>
@@ -3354,14 +3363,14 @@
       </c>
       <c r="D266" s="5"/>
     </row>
-    <row r="267" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B267" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C267" s="7">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B267" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C267">
         <v>1</v>
       </c>
-      <c r="D267" s="8"/>
+      <c r="D267" s="5"/>
     </row>
     <row r="268" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B268" s="4" t="s">
@@ -3372,95 +3381,98 @@
       </c>
       <c r="D268" s="5"/>
     </row>
-    <row r="269" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="270" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B270" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C270" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D270" s="3"/>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B269" s="4"/>
+      <c r="D269" s="5"/>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B270" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C270" t="s">
+        <v>112</v>
+      </c>
+      <c r="D270" s="5"/>
     </row>
     <row r="271" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B271" s="4" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C271" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="D271" s="5"/>
     </row>
-    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B272" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C272" t="b">
+    <row r="272" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B272" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C272" s="7">
         <v>1</v>
       </c>
-      <c r="D272" s="5"/>
+      <c r="D272" s="8"/>
     </row>
     <row r="273" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B273" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C273" t="s">
-        <v>68</v>
+        <v>10</v>
+      </c>
+      <c r="C273" t="b">
+        <v>0</v>
       </c>
       <c r="D273" s="5"/>
     </row>
-    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B274" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C274" t="b">
-        <v>1</v>
-      </c>
-      <c r="D274" s="5"/>
-    </row>
-    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B275" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C275" t="s">
-        <v>132</v>
-      </c>
-      <c r="D275" s="5"/>
+    <row r="274" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="275" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B275" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D275" s="3"/>
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B276" s="4"/>
+      <c r="B276" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C276" t="s">
+        <v>135</v>
+      </c>
       <c r="D276" s="5"/>
     </row>
     <row r="277" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B277" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C277" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="C277" t="b">
+        <v>1</v>
       </c>
       <c r="D277" s="5"/>
     </row>
     <row r="278" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B278" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C278" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="D278" s="5"/>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B279" s="4" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="C279" t="b">
+        <v>1</v>
       </c>
       <c r="D279" s="5"/>
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C280" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="C280" t="s">
+        <v>132</v>
       </c>
       <c r="D280" s="5"/>
     </row>
@@ -3473,7 +3485,7 @@
         <v>5</v>
       </c>
       <c r="C282" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="D282" s="5"/>
     </row>
@@ -3497,7 +3509,7 @@
         <v>10</v>
       </c>
       <c r="C285" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D285" s="5"/>
     </row>
@@ -3510,7 +3522,7 @@
         <v>5</v>
       </c>
       <c r="C287" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D287" s="5"/>
     </row>
@@ -3519,20 +3531,15 @@
         <v>7</v>
       </c>
       <c r="C288" t="s">
-        <v>12</v>
-      </c>
-      <c r="D288" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="289" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B289" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C289" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D289" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D288" s="5"/>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B289" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D289" s="5"/>
     </row>
     <row r="290" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B290" s="4" t="s">
@@ -3543,95 +3550,100 @@
       </c>
       <c r="D290" s="5"/>
     </row>
-    <row r="291" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="292" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B292" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D292" s="3"/>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B291" s="4"/>
+      <c r="D291" s="5"/>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B292" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C292" t="s">
+        <v>70</v>
+      </c>
+      <c r="D292" s="5"/>
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" s="4" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C293" t="s">
-        <v>135</v>
-      </c>
-      <c r="D293" s="5"/>
-    </row>
-    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B294" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C294" t="b">
-        <v>1</v>
-      </c>
-      <c r="D294" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D293" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B294" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C294" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D294" s="8"/>
     </row>
     <row r="295" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B295" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C295" t="s">
-        <v>68</v>
+        <v>10</v>
+      </c>
+      <c r="C295" t="b">
+        <v>0</v>
       </c>
       <c r="D295" s="5"/>
     </row>
-    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B296" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C296" t="b">
-        <v>1</v>
-      </c>
-      <c r="D296" s="5"/>
-    </row>
-    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B297" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C297" t="s">
-        <v>133</v>
-      </c>
-      <c r="D297" s="5"/>
+    <row r="296" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="297" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B297" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D297" s="3"/>
     </row>
     <row r="298" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B298" s="4"/>
+      <c r="B298" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C298" t="s">
+        <v>135</v>
+      </c>
       <c r="D298" s="5"/>
     </row>
     <row r="299" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B299" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C299" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="C299" t="b">
+        <v>1</v>
       </c>
       <c r="D299" s="5"/>
     </row>
     <row r="300" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B300" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C300" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="D300" s="5"/>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" s="4" t="s">
-        <v>9</v>
+        <v>78</v>
+      </c>
+      <c r="C301" t="b">
+        <v>1</v>
       </c>
       <c r="D301" s="5"/>
     </row>
     <row r="302" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B302" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C302" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="C302" t="s">
+        <v>133</v>
       </c>
       <c r="D302" s="5"/>
     </row>
@@ -3644,7 +3656,7 @@
         <v>5</v>
       </c>
       <c r="C304" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="D304" s="5"/>
     </row>
@@ -3668,7 +3680,7 @@
         <v>10</v>
       </c>
       <c r="C307" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D307" s="5"/>
     </row>
@@ -3681,7 +3693,7 @@
         <v>5</v>
       </c>
       <c r="C309" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D309" s="5"/>
     </row>
@@ -3690,20 +3702,15 @@
         <v>7</v>
       </c>
       <c r="C310" t="s">
-        <v>12</v>
-      </c>
-      <c r="D310" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="311" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B311" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C311" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D311" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="D310" s="5"/>
+    </row>
+    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B311" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D311" s="5"/>
     </row>
     <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" s="4" t="s">
@@ -3714,98 +3721,140 @@
       </c>
       <c r="D312" s="5"/>
     </row>
-    <row r="313" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="314" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B314" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C314" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D314" s="3"/>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B313" s="4"/>
+      <c r="D313" s="5"/>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B314" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C314" t="s">
+        <v>70</v>
+      </c>
+      <c r="D314" s="5"/>
     </row>
     <row r="315" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B315" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C315" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D315" s="5"/>
-    </row>
-    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B316" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C316" t="b">
-        <v>1</v>
-      </c>
-      <c r="D316" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C315" t="s">
+        <v>12</v>
+      </c>
+      <c r="D315" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="316" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B316" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C316" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D316" s="8"/>
     </row>
     <row r="317" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B317" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C317" s="12" t="s">
-        <v>136</v>
+        <v>10</v>
+      </c>
+      <c r="C317" t="b">
+        <v>0</v>
       </c>
       <c r="D317" s="5"/>
     </row>
-    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B318" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C318" t="b">
-        <v>1</v>
-      </c>
-      <c r="D318" s="5"/>
-    </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B319" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C319" t="s">
-        <v>134</v>
-      </c>
-      <c r="D319" s="5"/>
+    <row r="318" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="319" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B319" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C319" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D319" s="3"/>
     </row>
     <row r="320" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B320" s="4"/>
+      <c r="B320" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C320" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="D320" s="5"/>
     </row>
     <row r="321" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B321" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C321" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="C321" t="b">
+        <v>1</v>
       </c>
       <c r="D321" s="5"/>
     </row>
     <row r="322" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B322" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C322" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C322" s="12" t="s">
+        <v>136</v>
       </c>
       <c r="D322" s="5"/>
     </row>
-    <row r="323" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B323" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C323" s="7"/>
-      <c r="D323" s="8"/>
+    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B323" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C323" t="b">
+        <v>1</v>
+      </c>
+      <c r="D323" s="5"/>
     </row>
     <row r="324" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B324" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C324" t="b">
-        <v>0</v>
+        <v>114</v>
+      </c>
+      <c r="C324" t="s">
+        <v>134</v>
       </c>
       <c r="D324" s="5"/>
+    </row>
+    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B325" s="4"/>
+      <c r="D325" s="5"/>
+    </row>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B326" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C326" t="s">
+        <v>30</v>
+      </c>
+      <c r="D326" s="5"/>
+    </row>
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B327" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C327" t="s">
+        <v>8</v>
+      </c>
+      <c r="D327" s="5"/>
+    </row>
+    <row r="328" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B328" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C328" s="7"/>
+      <c r="D328" s="8"/>
+    </row>
+    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B329" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C329" t="b">
+        <v>0</v>
+      </c>
+      <c r="D329" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Aliquot and Pool blocks to suit new python code
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BCEBF1-1EEE-4AF9-B0BA-A6695F65D705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC246E4-DA09-482B-BF77-BCA1AE6AE83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="148">
   <si>
     <t>Step</t>
   </si>
@@ -244,9 +244,6 @@
     <t>55CBCD</t>
   </si>
   <si>
-    <t>Aspirate Location</t>
-  </si>
-  <si>
     <t>Start Position</t>
   </si>
   <si>
@@ -286,9 +283,6 @@
     <t>100,100 + 100</t>
   </si>
   <si>
-    <t>MAM/Low Artifact,HCP/Proteomics</t>
-  </si>
-  <si>
     <t>96 Well PCR Plate,96 Well UV Plate</t>
   </si>
   <si>
@@ -394,9 +388,6 @@
     <t>Load Volume</t>
   </si>
   <si>
-    <t>No,Dispense:10,Aspirate:10,Dispense:10;Aspirate:10</t>
-  </si>
-  <si>
     <t>Dispense:10</t>
   </si>
   <si>
@@ -473,6 +464,21 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>MAM/Low Artifact,HCP/Proteomics,Anjis Elution method</t>
+  </si>
+  <si>
+    <t>No,Dispense:10,Aspirate:10,Aspirate:10 + Dispense:10</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>95A17E</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsPause</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -608,8 +614,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,19 +1022,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:G329"/>
+  <dimension ref="B1:G326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="C283" sqref="C283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="74.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="21.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="10"/>
+    <col min="6" max="6" width="28.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="80" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1043,35 +1050,35 @@
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C4" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>28</v>
@@ -1081,62 +1088,62 @@
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" t="b">
+        <v>77</v>
+      </c>
+      <c r="C6" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" t="s">
-        <v>121</v>
+        <v>112</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="D7" s="5"/>
       <c r="F7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="D8" s="5"/>
       <c r="F8" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5"/>
@@ -1147,15 +1154,15 @@
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1164,47 +1171,47 @@
       </c>
       <c r="D11" s="5"/>
       <c r="F11" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="b">
+      <c r="C12" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="F13" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="5"/>
       <c r="F14" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>54</v>
@@ -1214,51 +1221,51 @@
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="7" t="s">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="5"/>
       <c r="F16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="F17" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="F17" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="G17" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1270,22 +1277,22 @@
       </c>
       <c r="D19" s="3"/>
       <c r="F19" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>54</v>
@@ -1295,7 +1302,7 @@
       <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C21" t="b">
+      <c r="C21" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="5"/>
@@ -1306,81 +1313,81 @@
       <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="b">
+        <v>77</v>
+      </c>
+      <c r="C23" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" t="s">
-        <v>122</v>
+        <v>112</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>119</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="F25" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
@@ -1391,62 +1398,62 @@
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C29" t="b">
+      <c r="C29" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="5"/>
       <c r="F29" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C31" t="s">
-        <v>115</v>
+      <c r="C31" s="10" t="s">
+        <v>113</v>
       </c>
       <c r="D31" s="5"/>
       <c r="F31" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>54</v>
@@ -1456,7 +1463,7 @@
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="5"/>
@@ -1467,89 +1474,89 @@
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C34" t="b">
+      <c r="C34" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="5"/>
       <c r="F34" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C36" t="s">
-        <v>116</v>
+      <c r="C36" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="D36" s="5"/>
       <c r="F36" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="5"/>
       <c r="F37" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="8"/>
+      <c r="D38" s="5"/>
       <c r="F38" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="5"/>
+    <row r="39" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="8"/>
       <c r="F39" s="4"/>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F40" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1561,52 +1568,52 @@
       </c>
       <c r="D41" s="3"/>
       <c r="F41" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="D42" s="5"/>
       <c r="F42" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C43" t="b">
+      <c r="C43" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="5"/>
       <c r="F43" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D44" s="5"/>
       <c r="F44" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>54</v>
@@ -1614,9 +1621,9 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" t="b">
+        <v>77</v>
+      </c>
+      <c r="C45" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D45" s="5"/>
@@ -1625,68 +1632,68 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" t="s">
-        <v>123</v>
+        <v>112</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="D46" s="5"/>
       <c r="F46" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="D47" s="5"/>
       <c r="F47" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D48" s="5"/>
       <c r="F48" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="F49" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="F49" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="5"/>
-      <c r="F50" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G50" s="5" t="s">
+      <c r="F50" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1694,7 +1701,7 @@
       <c r="B51" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C51" t="b">
+      <c r="C51" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D51" s="5"/>
@@ -1707,7 +1714,7 @@
       <c r="B53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D53" s="5"/>
@@ -1716,30 +1723,30 @@
       <c r="B54" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" s="7" t="s">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D55" s="8"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C56" t="b">
-        <v>0</v>
-      </c>
-      <c r="D56" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" s="8"/>
     </row>
     <row r="57" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1753,10 +1760,10 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C59" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="D59" s="5"/>
     </row>
@@ -1764,7 +1771,7 @@
       <c r="B60" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C60" t="b">
+      <c r="C60" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D60" s="5"/>
@@ -1773,33 +1780,28 @@
       <c r="B61" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="5"/>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C62" t="b">
+        <v>77</v>
+      </c>
+      <c r="C62" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C63" t="s">
-        <v>124</v>
-      </c>
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="6"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="8"/>
+    <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D63" s="8"/>
     </row>
     <row r="65" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -1813,10 +1815,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="C67" t="s">
-        <v>88</v>
       </c>
       <c r="D67" s="5"/>
     </row>
@@ -1824,7 +1826,7 @@
       <c r="B68" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C68" t="b">
+      <c r="C68" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D68" s="5"/>
@@ -1833,26 +1835,26 @@
       <c r="B69" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" t="b">
+        <v>77</v>
+      </c>
+      <c r="C70" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C71" t="s">
-        <v>125</v>
+        <v>112</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="D71" s="5"/>
     </row>
@@ -1864,7 +1866,7 @@
       <c r="B73" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D73" s="5"/>
@@ -1873,7 +1875,7 @@
       <c r="B74" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D74" s="5"/>
@@ -1888,7 +1890,7 @@
       <c r="B76" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C76" t="b">
+      <c r="C76" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D76" s="5"/>
@@ -1901,7 +1903,7 @@
       <c r="B78" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D78" s="5"/>
@@ -1910,7 +1912,7 @@
       <c r="B79" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D79" s="5"/>
@@ -1925,7 +1927,7 @@
       <c r="B81" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C81" t="b">
+      <c r="C81" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D81" s="5"/>
@@ -1938,8 +1940,8 @@
       <c r="B83" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C83" t="s">
-        <v>76</v>
+      <c r="C83" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="D83" s="5"/>
     </row>
@@ -1947,30 +1949,30 @@
       <c r="B84" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D85" s="8"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C86" t="b">
-        <v>0</v>
-      </c>
-      <c r="D86" s="5"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D86" s="8"/>
     </row>
     <row r="87" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -1984,10 +1986,10 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C89" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="C89" t="s">
-        <v>88</v>
       </c>
       <c r="D89" s="5"/>
     </row>
@@ -1995,7 +1997,7 @@
       <c r="B90" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C90" t="b">
+      <c r="C90" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D90" s="5"/>
@@ -2004,26 +2006,26 @@
       <c r="B91" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D91" s="5"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C92" t="b">
+        <v>77</v>
+      </c>
+      <c r="C92" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D92" s="5"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C93" t="s">
-        <v>126</v>
+        <v>112</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>123</v>
       </c>
       <c r="D93" s="5"/>
     </row>
@@ -2035,7 +2037,7 @@
       <c r="B95" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D95" s="5"/>
@@ -2044,7 +2046,7 @@
       <c r="B96" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D96" s="5"/>
@@ -2059,7 +2061,7 @@
       <c r="B98" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C98" t="b">
+      <c r="C98" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D98" s="5"/>
@@ -2072,7 +2074,7 @@
       <c r="B100" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D100" s="5"/>
@@ -2081,7 +2083,7 @@
       <c r="B101" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D101" s="5"/>
@@ -2096,7 +2098,7 @@
       <c r="B103" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C103" t="b">
+      <c r="C103" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D103" s="5"/>
@@ -2109,7 +2111,7 @@
       <c r="B105" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D105" s="5"/>
@@ -2118,7 +2120,7 @@
       <c r="B106" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D106" s="5"/>
@@ -2133,7 +2135,7 @@
       <c r="B108" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C108" t="b">
+      <c r="C108" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D108" s="5"/>
@@ -2146,7 +2148,7 @@
       <c r="B110" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D110" s="5"/>
@@ -2155,7 +2157,7 @@
       <c r="B111" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D111" s="5"/>
@@ -2170,7 +2172,7 @@
       <c r="B113" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C113" t="b">
+      <c r="C113" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D113" s="5"/>
@@ -2183,7 +2185,7 @@
       <c r="B115" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D115" s="5"/>
@@ -2192,7 +2194,7 @@
       <c r="B116" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D116" s="5"/>
@@ -2207,7 +2209,7 @@
       <c r="B118" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C118" t="b">
+      <c r="C118" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D118" s="5"/>
@@ -2220,7 +2222,7 @@
       <c r="B120" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D120" s="5"/>
@@ -2229,26 +2231,25 @@
       <c r="B121" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D121" s="5"/>
     </row>
-    <row r="122" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C122" s="7"/>
-      <c r="D122" s="8"/>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C123" t="b">
-        <v>0</v>
-      </c>
-      <c r="D123" s="5"/>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B123" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D123" s="8"/>
     </row>
     <row r="124" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="125" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -2256,16 +2257,16 @@
         <v>0</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D125" s="3"/>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C126" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="C126" t="s">
-        <v>88</v>
       </c>
       <c r="D126" s="5"/>
     </row>
@@ -2273,7 +2274,7 @@
       <c r="B127" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C127" t="b">
+      <c r="C127" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D127" s="5"/>
@@ -2282,26 +2283,26 @@
       <c r="B128" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D128" s="5"/>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C129" t="b">
+        <v>77</v>
+      </c>
+      <c r="C129" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D129" s="5"/>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C130" t="s">
-        <v>127</v>
+        <v>112</v>
+      </c>
+      <c r="C130" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="D130" s="5"/>
     </row>
@@ -2313,7 +2314,7 @@
       <c r="B132" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D132" s="5"/>
@@ -2322,7 +2323,7 @@
       <c r="B133" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D133" s="5" t="s">
@@ -2333,7 +2334,7 @@
       <c r="B134" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D134" s="5"/>
@@ -2342,7 +2343,7 @@
       <c r="B135" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C135" t="b">
+      <c r="C135" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D135" s="5"/>
@@ -2351,78 +2352,77 @@
       <c r="B136" s="4"/>
       <c r="D136" s="5"/>
     </row>
-    <row r="137" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C137" s="12" t="s">
-        <v>144</v>
+      <c r="C137" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="D137" s="5"/>
     </row>
-    <row r="138" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C138" s="12" t="s">
+      <c r="C138" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C139" s="12" t="s">
-        <v>145</v>
+      <c r="C139" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="D139" s="5"/>
     </row>
-    <row r="140" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C140" s="12" t="b">
+      <c r="C140" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D140" s="5"/>
     </row>
-    <row r="141" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="4"/>
       <c r="D141" s="5"/>
     </row>
-    <row r="142" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D142" s="5"/>
     </row>
-    <row r="143" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D143" s="5"/>
     </row>
-    <row r="144" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C144"/>
       <c r="D144" s="5"/>
     </row>
-    <row r="145" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C145" t="b">
+      <c r="C145" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D145" s="5"/>
@@ -2435,7 +2435,7 @@
       <c r="B147" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D147" s="5"/>
@@ -2444,28 +2444,28 @@
       <c r="B148" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D148" s="5"/>
     </row>
-    <row r="149" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C149" s="7">
-        <v>0</v>
-      </c>
-      <c r="D149" s="8"/>
-    </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C150" t="b">
-        <v>0</v>
-      </c>
-      <c r="D150" s="5"/>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" s="10">
+        <v>0</v>
+      </c>
+      <c r="D149" s="5"/>
+    </row>
+    <row r="150" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B150" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C150" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D150" s="8"/>
     </row>
     <row r="151" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="152" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -2473,16 +2473,16 @@
         <v>0</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D152" s="3"/>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C153" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="C153" t="s">
-        <v>88</v>
       </c>
       <c r="D153" s="5"/>
     </row>
@@ -2490,7 +2490,7 @@
       <c r="B154" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C154" t="b">
+      <c r="C154" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D154" s="5"/>
@@ -2499,26 +2499,26 @@
       <c r="B155" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D155" s="5"/>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C156" t="b">
+        <v>77</v>
+      </c>
+      <c r="C156" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D156" s="5"/>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C157" t="s">
-        <v>128</v>
+        <v>112</v>
+      </c>
+      <c r="C157" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="D157" s="5"/>
     </row>
@@ -2530,8 +2530,8 @@
       <c r="B159" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C159" t="s">
-        <v>117</v>
+      <c r="C159" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="D159" s="5"/>
     </row>
@@ -2539,7 +2539,7 @@
       <c r="B160" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D160" s="5"/>
@@ -2554,7 +2554,7 @@
       <c r="B162" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C162" t="b">
+      <c r="C162" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D162" s="5"/>
@@ -2567,8 +2567,8 @@
       <c r="B164" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C164" t="s">
-        <v>79</v>
+      <c r="C164" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="D164" s="5"/>
     </row>
@@ -2576,7 +2576,7 @@
       <c r="B165" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D165" s="5"/>
@@ -2591,7 +2591,7 @@
       <c r="B167" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C167" t="b">
+      <c r="C167" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D167" s="5"/>
@@ -2604,7 +2604,7 @@
       <c r="B169" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="10" t="s">
         <v>46</v>
       </c>
       <c r="D169" s="5"/>
@@ -2613,7 +2613,7 @@
       <c r="B170" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D170" s="5"/>
@@ -2628,7 +2628,7 @@
       <c r="B172" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C172" t="b">
+      <c r="C172" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D172" s="5"/>
@@ -2641,8 +2641,8 @@
       <c r="B174" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C174" t="s">
-        <v>118</v>
+      <c r="C174" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="D174" s="5"/>
     </row>
@@ -2650,39 +2650,38 @@
       <c r="B175" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C176" s="7"/>
-      <c r="D176" s="8"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D176" s="5"/>
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C177" t="b">
+      <c r="C177" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D177" s="5"/>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B178" s="10"/>
-      <c r="D178" s="10"/>
+      <c r="B178" s="4"/>
+      <c r="D178" s="5"/>
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C179" t="s">
-        <v>81</v>
+      <c r="C179" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="D179" s="5"/>
     </row>
@@ -2690,35 +2689,32 @@
       <c r="B180" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D180" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181" s="10" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="181" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B181" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C181" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D181" s="8"/>
-    </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B182" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C182" t="b">
-        <v>0</v>
-      </c>
-      <c r="D182" s="5"/>
-    </row>
-    <row r="183" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B183" s="10"/>
-      <c r="D183" s="10"/>
-    </row>
+      <c r="D181" s="5"/>
+    </row>
+    <row r="182" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C182" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D182" s="8"/>
+    </row>
+    <row r="183" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="184" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B184" s="1" t="s">
         <v>0</v>
@@ -2730,10 +2726,10 @@
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C185" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="C185" t="s">
-        <v>88</v>
       </c>
       <c r="D185" s="5"/>
     </row>
@@ -2741,7 +2737,7 @@
       <c r="B186" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C186" t="b">
+      <c r="C186" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D186" s="5"/>
@@ -2750,26 +2746,26 @@
       <c r="B187" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D187" s="5"/>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C188" t="b">
+        <v>77</v>
+      </c>
+      <c r="C188" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D188" s="5"/>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C189" t="s">
-        <v>129</v>
+        <v>112</v>
+      </c>
+      <c r="C189" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="D189" s="5"/>
     </row>
@@ -2781,7 +2777,7 @@
       <c r="B191" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D191" s="5"/>
@@ -2790,7 +2786,7 @@
       <c r="B192" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D192" s="5"/>
@@ -2805,7 +2801,7 @@
       <c r="B194" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C194" t="b">
+      <c r="C194" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D194" s="5"/>
@@ -2818,7 +2814,7 @@
       <c r="B196" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C196" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D196" s="5"/>
@@ -2827,7 +2823,7 @@
       <c r="B197" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C197" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D197" s="5"/>
@@ -2842,7 +2838,7 @@
       <c r="B199" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C199" t="b">
+      <c r="C199" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D199" s="5"/>
@@ -2855,7 +2851,7 @@
       <c r="B201" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C201" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D201" s="5"/>
@@ -2864,7 +2860,7 @@
       <c r="B202" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C202" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D202" s="5" t="s">
@@ -2881,7 +2877,7 @@
       <c r="B204" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C204" t="b">
+      <c r="C204" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D204" s="5"/>
@@ -2894,7 +2890,7 @@
       <c r="B206" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C206" t="s">
+      <c r="C206" s="10" t="s">
         <v>51</v>
       </c>
       <c r="D206" s="5"/>
@@ -2903,7 +2899,7 @@
       <c r="B207" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D207" s="5"/>
@@ -2918,7 +2914,7 @@
       <c r="B209" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C209" t="b">
+      <c r="C209" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D209" s="5"/>
@@ -2931,7 +2927,7 @@
       <c r="B211" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C211" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D211" s="5"/>
@@ -2940,7 +2936,7 @@
       <c r="B212" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D212" s="5" t="s">
@@ -2951,7 +2947,7 @@
       <c r="B213" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C213" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D213" s="5"/>
@@ -2960,7 +2956,7 @@
       <c r="B214" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C214" t="b">
+      <c r="C214" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D214" s="5"/>
@@ -2973,7 +2969,7 @@
       <c r="B216" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="10" t="s">
         <v>55</v>
       </c>
       <c r="D216" s="5"/>
@@ -2982,26 +2978,25 @@
       <c r="B217" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D217" s="5"/>
     </row>
-    <row r="218" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B218" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C218" s="7"/>
-      <c r="D218" s="8"/>
-    </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B219" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C219" t="b">
-        <v>0</v>
-      </c>
-      <c r="D219" s="5"/>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B218" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D218" s="5"/>
+    </row>
+    <row r="219" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B219" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C219" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D219" s="8"/>
     </row>
     <row r="220" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="221" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -3015,10 +3010,10 @@
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C222" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="C222" t="s">
-        <v>88</v>
       </c>
       <c r="D222" s="5"/>
     </row>
@@ -3026,7 +3021,7 @@
       <c r="B223" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C223" t="b">
+      <c r="C223" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D223" s="5"/>
@@ -3035,26 +3030,26 @@
       <c r="B224" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C224" s="10" t="s">
         <v>57</v>
       </c>
       <c r="D224" s="5"/>
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B225" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C225" t="b">
+        <v>77</v>
+      </c>
+      <c r="C225" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D225" s="5"/>
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C226" t="s">
-        <v>130</v>
+        <v>112</v>
+      </c>
+      <c r="C226" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="D226" s="5"/>
     </row>
@@ -3066,7 +3061,7 @@
       <c r="B228" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="10" t="s">
         <v>58</v>
       </c>
       <c r="D228" s="5"/>
@@ -3075,7 +3070,7 @@
       <c r="B229" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C229" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D229" s="5" t="s">
@@ -3086,7 +3081,7 @@
       <c r="B230" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C230" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D230" s="5"/>
@@ -3095,7 +3090,7 @@
       <c r="B231" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C231" t="b">
+      <c r="C231" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D231" s="5"/>
@@ -3108,7 +3103,7 @@
       <c r="B233" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C233" s="10" t="s">
         <v>59</v>
       </c>
       <c r="D233" s="5"/>
@@ -3117,7 +3112,7 @@
       <c r="B234" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C234" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D234" s="5"/>
@@ -3132,7 +3127,7 @@
       <c r="B236" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C236" t="b">
+      <c r="C236" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D236" s="5"/>
@@ -3145,7 +3140,7 @@
       <c r="B238" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C238" s="10" t="s">
         <v>60</v>
       </c>
       <c r="D238" s="5"/>
@@ -3154,26 +3149,25 @@
       <c r="B239" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C239" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D239" s="5"/>
     </row>
-    <row r="240" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B240" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C240" s="7"/>
-      <c r="D240" s="8"/>
-    </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B241" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C241" t="b">
-        <v>0</v>
-      </c>
-      <c r="D241" s="5"/>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D240" s="5"/>
+    </row>
+    <row r="241" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B241" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C241" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D241" s="8"/>
     </row>
     <row r="242" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="243" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -3187,10 +3181,10 @@
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C244" s="10" t="s">
         <v>86</v>
-      </c>
-      <c r="C244" t="s">
-        <v>88</v>
       </c>
       <c r="D244" s="5"/>
     </row>
@@ -3198,7 +3192,7 @@
       <c r="B245" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C245" t="b">
+      <c r="C245" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D245" s="5"/>
@@ -3207,26 +3201,26 @@
       <c r="B246" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C246" s="10" t="s">
         <v>62</v>
       </c>
       <c r="D246" s="5"/>
     </row>
     <row r="247" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B247" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C247" t="b">
+        <v>77</v>
+      </c>
+      <c r="C247" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D247" s="5"/>
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C248" t="s">
-        <v>131</v>
+        <v>112</v>
+      </c>
+      <c r="C248" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="D248" s="5"/>
     </row>
@@ -3238,7 +3232,7 @@
       <c r="B250" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C250" t="s">
+      <c r="C250" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D250" s="5"/>
@@ -3247,7 +3241,7 @@
       <c r="B251" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C251" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D251" s="5"/>
@@ -3262,7 +3256,7 @@
       <c r="B253" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C253" t="b">
+      <c r="C253" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D253" s="5"/>
@@ -3275,7 +3269,7 @@
       <c r="B255" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C255" s="10" t="s">
         <v>64</v>
       </c>
       <c r="D255" s="5"/>
@@ -3284,7 +3278,7 @@
       <c r="B256" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C256" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D256" s="5"/>
@@ -3299,7 +3293,7 @@
       <c r="B258" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C258" t="b">
+      <c r="C258" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D258" s="5"/>
@@ -3312,7 +3306,7 @@
       <c r="B260" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C260" t="s">
+      <c r="C260" s="10" t="s">
         <v>65</v>
       </c>
       <c r="D260" s="5"/>
@@ -3321,7 +3315,7 @@
       <c r="B261" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C261" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D261" s="5"/>
@@ -3336,7 +3330,7 @@
       <c r="B263" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C263" t="b">
+      <c r="C263" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D263" s="5"/>
@@ -3349,7 +3343,7 @@
       <c r="B265" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C265" t="s">
+      <c r="C265" s="10" t="s">
         <v>66</v>
       </c>
       <c r="D265" s="5"/>
@@ -3358,7 +3352,7 @@
       <c r="B266" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C266" t="s">
+      <c r="C266" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D266" s="5"/>
@@ -3367,7 +3361,7 @@
       <c r="B267" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C267">
+      <c r="C267" s="10">
         <v>1</v>
       </c>
       <c r="D267" s="5"/>
@@ -3376,7 +3370,7 @@
       <c r="B268" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C268" t="b">
+      <c r="C268" s="10" t="b">
         <v>0</v>
       </c>
       <c r="D268" s="5"/>
@@ -3389,8 +3383,8 @@
       <c r="B270" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C270" t="s">
-        <v>112</v>
+      <c r="C270" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="D270" s="5"/>
     </row>
@@ -3398,28 +3392,28 @@
       <c r="B271" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C271" t="s">
+      <c r="C271" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D271" s="5"/>
     </row>
-    <row r="272" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B272" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C272" s="7">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B272" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C272" s="10">
         <v>1</v>
       </c>
-      <c r="D272" s="8"/>
-    </row>
-    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B273" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C273" t="b">
-        <v>0</v>
-      </c>
-      <c r="D273" s="5"/>
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B273" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C273" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D273" s="8"/>
     </row>
     <row r="274" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="275" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -3433,10 +3427,10 @@
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C276" t="s">
-        <v>135</v>
+        <v>84</v>
+      </c>
+      <c r="C276" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="D276" s="5"/>
     </row>
@@ -3444,7 +3438,7 @@
       <c r="B277" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C277" t="b">
+      <c r="C277" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D277" s="5"/>
@@ -3453,26 +3447,26 @@
       <c r="B278" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C278" t="s">
+      <c r="C278" s="10" t="s">
         <v>68</v>
       </c>
       <c r="D278" s="5"/>
     </row>
     <row r="279" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B279" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C279" t="b">
+        <v>77</v>
+      </c>
+      <c r="C279" s="10" t="b">
         <v>1</v>
       </c>
       <c r="D279" s="5"/>
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C280" t="s">
-        <v>132</v>
+        <v>112</v>
+      </c>
+      <c r="C280" s="10" t="s">
+        <v>129</v>
       </c>
       <c r="D280" s="5"/>
     </row>
@@ -3484,8 +3478,8 @@
       <c r="B282" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C282" t="s">
-        <v>27</v>
+      <c r="C282" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="D282" s="5"/>
     </row>
@@ -3493,368 +3487,348 @@
       <c r="B283" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C283" t="s">
-        <v>8</v>
-      </c>
-      <c r="D283" s="5"/>
+      <c r="C283" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D283" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="284" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B284" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C284" s="10" t="s">
+        <v>71</v>
+      </c>
       <c r="D284" s="5"/>
     </row>
-    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B285" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C285" t="b">
-        <v>1</v>
-      </c>
-      <c r="D285" s="5"/>
-    </row>
-    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B286" s="4"/>
-      <c r="D286" s="5"/>
-    </row>
-    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B287" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C287" t="s">
-        <v>69</v>
-      </c>
-      <c r="D287" s="5"/>
+    <row r="285" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B285" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C285" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D285" s="8"/>
+    </row>
+    <row r="286" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="287" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B287" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D287" s="3"/>
     </row>
     <row r="288" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B288" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C288" t="s">
-        <v>8</v>
+        <v>84</v>
+      </c>
+      <c r="C288" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="D288" s="5"/>
     </row>
     <row r="289" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B289" s="4" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="C289" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D289" s="5"/>
     </row>
     <row r="290" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B290" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C290" t="b">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="C290" s="10" t="s">
+        <v>68</v>
       </c>
       <c r="D290" s="5"/>
     </row>
     <row r="291" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B291" s="4"/>
+      <c r="B291" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C291" s="10" t="b">
+        <v>1</v>
+      </c>
       <c r="D291" s="5"/>
     </row>
     <row r="292" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B292" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C292" t="s">
-        <v>70</v>
+        <v>112</v>
+      </c>
+      <c r="C292" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="D292" s="5"/>
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B293" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C293" t="s">
-        <v>12</v>
-      </c>
-      <c r="D293" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="294" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B294" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C294" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D294" s="8"/>
+      <c r="B293" s="4"/>
+      <c r="D293" s="5"/>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B294" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C294" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D294" s="5"/>
     </row>
     <row r="295" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B295" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C295" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C295" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D295" s="5"/>
     </row>
-    <row r="296" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="297" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B297" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D297" s="3"/>
+    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B296" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D296" s="5"/>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B297" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C297" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D297" s="5"/>
     </row>
     <row r="298" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B298" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C298" t="s">
-        <v>135</v>
-      </c>
+      <c r="B298" s="4"/>
       <c r="D298" s="5"/>
     </row>
     <row r="299" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B299" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C299" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C299" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="D299" s="5"/>
     </row>
     <row r="300" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B300" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C300" t="s">
-        <v>68</v>
-      </c>
-      <c r="D300" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C300" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D300" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C301" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C301" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D301" s="5"/>
     </row>
-    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B302" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C302" t="s">
-        <v>133</v>
-      </c>
-      <c r="D302" s="5"/>
-    </row>
-    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B303" s="4"/>
-      <c r="D303" s="5"/>
-    </row>
-    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B304" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C304" t="s">
-        <v>27</v>
-      </c>
-      <c r="D304" s="5"/>
+    <row r="302" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B302" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C302" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D302" s="8"/>
+    </row>
+    <row r="303" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="304" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B304" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D304" s="3"/>
     </row>
     <row r="305" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B305" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C305" t="s">
-        <v>8</v>
+        <v>84</v>
+      </c>
+      <c r="C305" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="D305" s="5"/>
     </row>
     <row r="306" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B306" s="4" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="C306" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D306" s="5"/>
     </row>
     <row r="307" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B307" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C307" t="b">
+        <v>3</v>
+      </c>
+      <c r="C307" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D307" s="5"/>
+    </row>
+    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B308" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C308" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="D307" s="5"/>
-    </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B308" s="4"/>
       <c r="D308" s="5"/>
     </row>
     <row r="309" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B309" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C309" t="s">
-        <v>74</v>
+        <v>112</v>
+      </c>
+      <c r="C309" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="D309" s="5"/>
     </row>
     <row r="310" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B310" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C310" t="s">
-        <v>8</v>
-      </c>
+      <c r="B310" s="4"/>
       <c r="D310" s="5"/>
     </row>
     <row r="311" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B311" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="C311" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D311" s="5"/>
     </row>
     <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C312" t="b">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C312" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D312" s="5"/>
     </row>
     <row r="313" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B313" s="4"/>
+      <c r="B313" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D313" s="5"/>
     </row>
-    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B314" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C314" t="s">
-        <v>70</v>
-      </c>
-      <c r="D314" s="5"/>
-    </row>
-    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B315" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C315" t="s">
-        <v>12</v>
-      </c>
-      <c r="D315" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="316" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B316" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C316" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D316" s="8"/>
+    <row r="314" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B314" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C314" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D314" s="8"/>
+    </row>
+    <row r="315" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="316" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B316" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D316" s="3"/>
     </row>
     <row r="317" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B317" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C317" t="b">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="C317" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="D317" s="5"/>
     </row>
-    <row r="318" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="319" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B319" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C319" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D319" s="3"/>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B318" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C318" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D318" s="5"/>
+    </row>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B319" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C319" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D319" s="5"/>
     </row>
     <row r="320" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B320" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C320" s="11" t="s">
-        <v>88</v>
+        <v>77</v>
+      </c>
+      <c r="C320" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D320" s="5"/>
     </row>
     <row r="321" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B321" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C321" t="b">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="C321" s="10" t="s">
+        <v>147</v>
       </c>
       <c r="D321" s="5"/>
     </row>
     <row r="322" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B322" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C322" s="12" t="s">
-        <v>136</v>
-      </c>
+      <c r="B322" s="4"/>
       <c r="D322" s="5"/>
     </row>
     <row r="323" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B323" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C323" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C323" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="D323" s="5"/>
     </row>
     <row r="324" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B324" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C324" t="s">
-        <v>134</v>
+        <v>7</v>
+      </c>
+      <c r="C324" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="D324" s="5"/>
     </row>
     <row r="325" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B325" s="4"/>
+      <c r="B325" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D325" s="5"/>
     </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B326" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C326" t="s">
-        <v>30</v>
-      </c>
-      <c r="D326" s="5"/>
-    </row>
-    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B327" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C327" t="s">
-        <v>8</v>
-      </c>
-      <c r="D327" s="5"/>
-    </row>
-    <row r="328" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B328" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C328" s="7"/>
-      <c r="D328" s="8"/>
-    </row>
-    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B329" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C329" t="b">
-        <v>0</v>
-      </c>
-      <c r="D329" s="5"/>
+    <row r="326" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B326" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C326" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D326" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3866,7 +3840,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updating the Serial Dilution originally made for Kate to also suit Ron.
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC246E4-DA09-482B-BF77-BCA1AE6AE83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A06896-EBED-459B-9825-7E5C1D7D4C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="157">
   <si>
     <t>Step</t>
   </si>
@@ -479,6 +479,33 @@
   </si>
   <si>
     <t>BlockDescriptionsPause</t>
+  </si>
+  <si>
+    <t>Serial Dilution</t>
+  </si>
+  <si>
+    <t>BlockDescriptionsSerialDilution</t>
+  </si>
+  <si>
+    <t>Max Dilution Factor (x)</t>
+  </si>
+  <si>
+    <t>Aspirate Location</t>
+  </si>
+  <si>
+    <t>Follow Starting and Target Concentration,Enter Numeric Value</t>
+  </si>
+  <si>
+    <t>Follow Starting and Target Concentration</t>
+  </si>
+  <si>
+    <t>Dilution Method</t>
+  </si>
+  <si>
+    <t>Use All Wells,Use Only Required Wells</t>
+  </si>
+  <si>
+    <t>Use Only Required Wells</t>
   </si>
 </sst>
 </file>
@@ -1022,17 +1049,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:G326"/>
+  <dimension ref="B1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
-      <selection activeCell="C283" sqref="C283"/>
+    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
+      <selection activeCell="C373" sqref="C373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="10"/>
     <col min="2" max="2" width="21.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="79.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="10"/>
     <col min="6" max="6" width="28.7109375" style="10" bestFit="1" customWidth="1"/>
@@ -3479,7 +3506,7 @@
         <v>5</v>
       </c>
       <c r="C282" s="10" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="D282" s="5"/>
     </row>
@@ -3488,119 +3515,119 @@
         <v>7</v>
       </c>
       <c r="C283" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D283" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D283" s="5"/>
     </row>
     <row r="284" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B284" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C284" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="D284" s="5"/>
     </row>
-    <row r="285" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B285" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C285" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D285" s="8"/>
-    </row>
-    <row r="286" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="287" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B287" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C287" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D287" s="3"/>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B285" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C285" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D285" s="5"/>
+    </row>
+    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B286" s="4"/>
+      <c r="D286" s="5"/>
+    </row>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B287" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C287" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D287" s="5"/>
     </row>
     <row r="288" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B288" s="4" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C288" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D288" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D288" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="289" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B289" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C289" s="10" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C289" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D289" s="5"/>
     </row>
-    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B290" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C290" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D290" s="5"/>
-    </row>
-    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B291" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C291" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D291" s="5"/>
-    </row>
-    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B292" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C292" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D292" s="5"/>
+    <row r="290" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B290" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C290" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D290" s="8"/>
+    </row>
+    <row r="291" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="292" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B292" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D292" s="3"/>
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B293" s="4"/>
+      <c r="B293" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C293" s="10" t="s">
+        <v>132</v>
+      </c>
       <c r="D293" s="5"/>
     </row>
     <row r="294" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B294" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C294" s="10" t="s">
-        <v>73</v>
+        <v>2</v>
+      </c>
+      <c r="C294" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D294" s="5"/>
     </row>
     <row r="295" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B295" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C295" s="10" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="D295" s="5"/>
     </row>
     <row r="296" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B296" s="4" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+      <c r="C296" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D296" s="5"/>
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C297" s="10" t="b">
-        <v>0</v>
+        <v>112</v>
+      </c>
+      <c r="C297" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="D297" s="5"/>
     </row>
@@ -3613,7 +3640,7 @@
         <v>5</v>
       </c>
       <c r="C299" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D299" s="5"/>
     </row>
@@ -3622,213 +3649,574 @@
         <v>7</v>
       </c>
       <c r="C300" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D300" s="5" t="s">
-        <v>70</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D300" s="5"/>
     </row>
     <row r="301" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B301" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C301" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="D301" s="5"/>
     </row>
-    <row r="302" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B302" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C302" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D302" s="8"/>
-    </row>
-    <row r="303" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="304" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B304" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C304" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D304" s="3"/>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B302" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C302" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D302" s="5"/>
+    </row>
+    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B303" s="4"/>
+      <c r="D303" s="5"/>
+    </row>
+    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B304" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C304" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D304" s="5"/>
     </row>
     <row r="305" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B305" s="4" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C305" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D305" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D305" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="306" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B306" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C306" s="10" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C306" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D306" s="5"/>
     </row>
-    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B307" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C307" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="D307" s="5"/>
-    </row>
-    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B308" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C308" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D308" s="5"/>
-    </row>
-    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B309" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C309" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="D309" s="5"/>
+    <row r="307" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B307" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C307" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D307" s="8"/>
+    </row>
+    <row r="308" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="309" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B309" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C309" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D309" s="3"/>
     </row>
     <row r="310" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B310" s="4"/>
+      <c r="B310" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C310" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="D310" s="5"/>
     </row>
     <row r="311" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B311" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C311" s="10" t="s">
-        <v>30</v>
+        <v>2</v>
+      </c>
+      <c r="C311" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D311" s="5"/>
     </row>
     <row r="312" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B312" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C312" s="10" t="s">
-        <v>8</v>
+        <v>133</v>
       </c>
       <c r="D312" s="5"/>
     </row>
     <row r="313" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B313" s="4" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+      <c r="C313" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D313" s="5"/>
     </row>
-    <row r="314" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B314" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C314" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D314" s="8"/>
-    </row>
-    <row r="315" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="316" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B316" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D316" s="3"/>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B314" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C314" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D314" s="5"/>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B315" s="4"/>
+      <c r="D315" s="5"/>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B316" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C316" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D316" s="5"/>
     </row>
     <row r="317" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B317" s="4" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C317" s="10" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="D317" s="5"/>
     </row>
     <row r="318" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B318" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C318" s="10" t="b">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D318" s="5"/>
     </row>
-    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B319" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C319" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D319" s="5"/>
-    </row>
-    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B320" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C320" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D320" s="5"/>
-    </row>
-    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B321" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C321" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D321" s="5"/>
+    <row r="319" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B319" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C319" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D319" s="8"/>
+    </row>
+    <row r="320" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="321" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B321" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D321" s="3"/>
     </row>
     <row r="322" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B322" s="4"/>
+      <c r="B322" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C322" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="D322" s="5"/>
     </row>
     <row r="323" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B323" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C323" s="10" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="C323" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D323" s="5"/>
     </row>
     <row r="324" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B324" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C324" s="10" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="D324" s="5"/>
     </row>
     <row r="325" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B325" s="4" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+      <c r="C325" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D325" s="5"/>
     </row>
-    <row r="326" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B326" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C326" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D326" s="8"/>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B326" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C326" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D326" s="5"/>
+    </row>
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B327" s="4"/>
+      <c r="D327" s="5"/>
+    </row>
+    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B328" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C328" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D328" s="5"/>
+    </row>
+    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B329" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C329" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D329" s="5"/>
+    </row>
+    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B330" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D330" s="5"/>
+    </row>
+    <row r="331" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B331" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C331" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D331" s="8"/>
+    </row>
+    <row r="332" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="333" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B333" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D333" s="3"/>
+    </row>
+    <row r="334" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B334" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C334" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D334" s="5"/>
+    </row>
+    <row r="335" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B335" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C335" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D335" s="5"/>
+    </row>
+    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B336" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C336" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D336" s="5"/>
+    </row>
+    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B337" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C337" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D337" s="5"/>
+    </row>
+    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B338" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C338" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D338" s="5"/>
+    </row>
+    <row r="339" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B339" s="4"/>
+      <c r="D339" s="5"/>
+    </row>
+    <row r="340" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B340" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C340" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D340" s="5"/>
+    </row>
+    <row r="341" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B341" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C341" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D341" s="5"/>
+    </row>
+    <row r="342" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B342" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D342" s="5"/>
+    </row>
+    <row r="343" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B343" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C343" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D343" s="5"/>
+    </row>
+    <row r="344" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B344" s="4"/>
+      <c r="D344" s="5"/>
+    </row>
+    <row r="345" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B345" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C345" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D345" s="5"/>
+    </row>
+    <row r="346" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B346" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C346" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D346" s="5"/>
+    </row>
+    <row r="347" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B347" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D347" s="5"/>
+    </row>
+    <row r="348" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B348" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C348" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D348" s="5"/>
+    </row>
+    <row r="349" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B349" s="4"/>
+      <c r="D349" s="5"/>
+    </row>
+    <row r="350" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B350" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C350" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D350" s="5"/>
+    </row>
+    <row r="351" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B351" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C351" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D351" s="5"/>
+    </row>
+    <row r="352" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B352" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D352" s="5"/>
+    </row>
+    <row r="353" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B353" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C353" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D353" s="5"/>
+    </row>
+    <row r="354" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B354" s="4"/>
+      <c r="D354" s="5"/>
+    </row>
+    <row r="355" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B355" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C355" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D355" s="5"/>
+    </row>
+    <row r="356" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B356" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C356" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D356" s="5"/>
+    </row>
+    <row r="357" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B357" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D357" s="5"/>
+    </row>
+    <row r="358" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B358" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C358" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D358" s="5"/>
+    </row>
+    <row r="359" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B359" s="4"/>
+      <c r="D359" s="5"/>
+    </row>
+    <row r="360" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B360" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C360" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D360" s="5"/>
+    </row>
+    <row r="361" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B361" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C361" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D361" s="5"/>
+    </row>
+    <row r="362" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B362" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D362" s="5"/>
+    </row>
+    <row r="363" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B363" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C363" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D363" s="5"/>
+    </row>
+    <row r="364" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B364" s="4"/>
+      <c r="D364" s="5"/>
+    </row>
+    <row r="365" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B365" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C365" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D365" s="5"/>
+    </row>
+    <row r="366" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B366" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C366" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D366" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="367" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B367" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C367" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D367" s="5"/>
+    </row>
+    <row r="368" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B368" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C368" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D368" s="5"/>
+    </row>
+    <row r="369" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B369" s="4"/>
+      <c r="D369" s="5"/>
+    </row>
+    <row r="370" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B370" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C370" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D370" s="5"/>
+    </row>
+    <row r="371" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B371" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C371" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D371" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="372" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B372" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C372" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D372" s="5"/>
+    </row>
+    <row r="373" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B373" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C373" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D373" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished Testing on Hamilton. Everything works. Now to create a super method and test for real.
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A06896-EBED-459B-9825-7E5C1D7D4C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8348608E-5F43-40B6-B68D-F4DE31EC6DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="4380" yWindow="630" windowWidth="21285" windowHeight="11385" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="158">
   <si>
     <t>Step</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>Use Only Required Wells</t>
+  </si>
+  <si>
+    <t>Max Dilution Steps</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1052,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:G373"/>
+  <dimension ref="B1:G378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
-      <selection activeCell="C373" sqref="C373"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="D372" sqref="D372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4185,7 +4188,7 @@
         <v>5</v>
       </c>
       <c r="C370" s="10" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D370" s="5"/>
     </row>
@@ -4194,29 +4197,66 @@
         <v>7</v>
       </c>
       <c r="C371" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D371" s="5" t="s">
-        <v>155</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D371" s="5"/>
     </row>
     <row r="372" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B372" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C372" s="10" t="s">
+      <c r="D372" s="5"/>
+    </row>
+    <row r="373" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B373" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C373" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D373" s="5"/>
+    </row>
+    <row r="374" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B374" s="4"/>
+      <c r="D374" s="5"/>
+    </row>
+    <row r="375" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B375" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C375" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D375" s="5"/>
+    </row>
+    <row r="376" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B376" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C376" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D376" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="377" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B377" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C377" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D372" s="5"/>
-    </row>
-    <row r="373" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B373" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C373" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D373" s="8"/>
+      <c r="D377" s="5"/>
+    </row>
+    <row r="378" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B378" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C378" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D378" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Trying to fix incubation...
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8348608E-5F43-40B6-B68D-F4DE31EC6DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF081B-8AD8-4890-9A0C-86875D34AE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="630" windowWidth="21285" windowHeight="11385" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="158">
   <si>
     <t>Step</t>
   </si>
@@ -1052,10 +1052,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:G378"/>
+  <dimension ref="B1:G383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
-      <selection activeCell="D372" sqref="D372"/>
+    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
+      <selection activeCell="C319" sqref="C319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3777,7 +3777,7 @@
         <v>5</v>
       </c>
       <c r="C316" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D316" s="5"/>
     </row>
@@ -3796,196 +3796,196 @@
       </c>
       <c r="D318" s="5"/>
     </row>
-    <row r="319" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B319" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C319" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D319" s="8"/>
-    </row>
-    <row r="320" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="321" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B321" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C321" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D321" s="3"/>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B319" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C319" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D319" s="5"/>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B320" s="4"/>
+      <c r="D320" s="5"/>
+    </row>
+    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B321" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C321" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D321" s="5"/>
     </row>
     <row r="322" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B322" s="4" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C322" s="10" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="D322" s="5"/>
     </row>
     <row r="323" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B323" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C323" s="10" t="b">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D323" s="5"/>
     </row>
-    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B324" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C324" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D324" s="5"/>
-    </row>
-    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B325" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C325" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D325" s="5"/>
-    </row>
-    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B326" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C326" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D326" s="5"/>
+    <row r="324" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B324" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C324" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D324" s="8"/>
+    </row>
+    <row r="325" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="326" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B326" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D326" s="3"/>
     </row>
     <row r="327" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B327" s="4"/>
+      <c r="B327" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C327" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="D327" s="5"/>
     </row>
     <row r="328" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B328" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C328" s="10" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="C328" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D328" s="5"/>
     </row>
     <row r="329" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B329" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C329" s="10" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="D329" s="5"/>
     </row>
     <row r="330" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B330" s="4" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+      <c r="C330" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D330" s="5"/>
     </row>
-    <row r="331" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B331" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C331" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D331" s="8"/>
-    </row>
-    <row r="332" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="333" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B333" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C333" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D333" s="3"/>
+    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B331" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C331" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D331" s="5"/>
+    </row>
+    <row r="332" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B332" s="4"/>
+      <c r="D332" s="5"/>
+    </row>
+    <row r="333" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B333" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C333" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D333" s="5"/>
     </row>
     <row r="334" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B334" s="4" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C334" s="10" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="D334" s="5"/>
     </row>
     <row r="335" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B335" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C335" s="10" t="b">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D335" s="5"/>
     </row>
-    <row r="336" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B336" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C336" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D336" s="5"/>
-    </row>
-    <row r="337" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B337" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C337" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D337" s="5"/>
-    </row>
-    <row r="338" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B338" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C338" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="D338" s="5"/>
+    <row r="336" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B336" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C336" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D336" s="8"/>
+    </row>
+    <row r="337" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="338" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B338" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C338" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D338" s="3"/>
     </row>
     <row r="339" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B339" s="4"/>
+      <c r="B339" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C339" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="D339" s="5"/>
     </row>
     <row r="340" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B340" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C340" s="10" t="s">
-        <v>27</v>
+        <v>2</v>
+      </c>
+      <c r="C340" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D340" s="5"/>
     </row>
     <row r="341" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B341" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C341" s="10" t="s">
-        <v>8</v>
+        <v>146</v>
       </c>
       <c r="D341" s="5"/>
     </row>
     <row r="342" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B342" s="4" t="s">
-        <v>9</v>
+        <v>77</v>
+      </c>
+      <c r="C342" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="D342" s="5"/>
     </row>
     <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C343" s="10" t="b">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="C343" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="D343" s="5"/>
     </row>
@@ -3998,7 +3998,7 @@
         <v>5</v>
       </c>
       <c r="C345" s="10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D345" s="5"/>
     </row>
@@ -4035,7 +4035,7 @@
         <v>5</v>
       </c>
       <c r="C350" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D350" s="5"/>
     </row>
@@ -4059,7 +4059,7 @@
         <v>10</v>
       </c>
       <c r="C353" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D353" s="5"/>
     </row>
@@ -4072,7 +4072,7 @@
         <v>5</v>
       </c>
       <c r="C355" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D355" s="5"/>
     </row>
@@ -4109,7 +4109,7 @@
         <v>5</v>
       </c>
       <c r="C360" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D360" s="5"/>
     </row>
@@ -4146,7 +4146,7 @@
         <v>5</v>
       </c>
       <c r="C365" s="10" t="s">
-        <v>150</v>
+        <v>37</v>
       </c>
       <c r="D365" s="5"/>
     </row>
@@ -4155,18 +4155,13 @@
         <v>7</v>
       </c>
       <c r="C366" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D366" s="5" t="s">
-        <v>152</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D366" s="5"/>
     </row>
     <row r="367" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B367" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C367" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="D367" s="5"/>
     </row>
@@ -4188,7 +4183,7 @@
         <v>5</v>
       </c>
       <c r="C370" s="10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D370" s="5"/>
     </row>
@@ -4197,13 +4192,18 @@
         <v>7</v>
       </c>
       <c r="C371" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D371" s="5"/>
+        <v>41</v>
+      </c>
+      <c r="D371" s="5" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="372" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B372" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="C372" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="D372" s="5"/>
     </row>
@@ -4225,7 +4225,7 @@
         <v>5</v>
       </c>
       <c r="C375" s="10" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D375" s="5"/>
     </row>
@@ -4234,29 +4234,66 @@
         <v>7</v>
       </c>
       <c r="C376" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D376" s="5" t="s">
-        <v>155</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D376" s="5"/>
     </row>
     <row r="377" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B377" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C377" s="10" t="s">
+      <c r="D377" s="5"/>
+    </row>
+    <row r="378" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B378" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C378" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D378" s="5"/>
+    </row>
+    <row r="379" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B379" s="4"/>
+      <c r="D379" s="5"/>
+    </row>
+    <row r="380" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B380" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C380" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D380" s="5"/>
+    </row>
+    <row r="381" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B381" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C381" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D381" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="382" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B382" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C382" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D377" s="5"/>
-    </row>
-    <row r="378" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B378" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C378" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D378" s="8"/>
+      <c r="D382" s="5"/>
+    </row>
+    <row r="383" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B383" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C383" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D383" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Pyhton Config, and Modules config. Now I need to finish deck layout and deck loading.
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF081B-8AD8-4890-9A0C-86875D34AE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28213924-A6E0-4556-A925-E5731ABCE4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -1054,8 +1054,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="C319" sqref="C319"/>
+    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="C343" sqref="C343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3241,7 +3241,7 @@
         <v>77</v>
       </c>
       <c r="C247" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D247" s="5"/>
     </row>
@@ -3976,7 +3976,7 @@
         <v>77</v>
       </c>
       <c r="C342" s="10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D342" s="5"/>
     </row>

</xml_diff>

<commit_message>
Adding starstedt tube as plate option
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF081B-8AD8-4890-9A0C-86875D34AE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECB00FF-7B29-4440-A909-7A59FFCBF6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>100,100 + 100</t>
   </si>
   <si>
-    <t>96 Well PCR Plate,96 Well UV Plate</t>
-  </si>
-  <si>
     <t>MAM/Low Artifact</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>Max Dilution Steps</t>
+  </si>
+  <si>
+    <t>96 Well PCR Plate,96 Well UV Plate,56 Well Starstedt 200uL Plate</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1054,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="C319" sqref="C319"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,23 +1080,23 @@
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>28</v>
@@ -1123,10 +1123,10 @@
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1138,35 +1138,35 @@
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="D8" s="5"/>
       <c r="F8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1189,10 +1189,10 @@
       </c>
       <c r="D10" s="5"/>
       <c r="F10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
       </c>
       <c r="D11" s="5"/>
       <c r="F11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -1216,20 +1216,20 @@
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="F13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="D14" s="5"/>
       <c r="F14" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>54</v>
@@ -1255,7 +1255,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
@@ -1269,10 +1269,10 @@
       </c>
       <c r="D16" s="5"/>
       <c r="F16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1284,18 +1284,18 @@
       </c>
       <c r="D17" s="8"/>
       <c r="F17" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1307,22 +1307,22 @@
       </c>
       <c r="D19" s="3"/>
       <c r="F19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>54</v>
@@ -1348,10 +1348,10 @@
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1363,35 +1363,35 @@
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="F25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1403,10 +1403,10 @@
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1417,7 +1417,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
@@ -1428,10 +1428,10 @@
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1443,20 +1443,20 @@
       </c>
       <c r="D29" s="5"/>
       <c r="F29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1464,14 +1464,14 @@
         <v>5</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D31" s="5"/>
       <c r="F31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>54</v>
@@ -1509,20 +1509,20 @@
       </c>
       <c r="D34" s="5"/>
       <c r="F34" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1530,14 +1530,14 @@
         <v>5</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="5"/>
       <c r="F36" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1549,10 +1549,10 @@
       </c>
       <c r="D37" s="5"/>
       <c r="F37" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="D38" s="5"/>
       <c r="F38" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>54</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F40" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1598,25 +1598,25 @@
       </c>
       <c r="D41" s="3"/>
       <c r="F41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D42" s="5"/>
       <c r="F42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -1628,10 +1628,10 @@
       </c>
       <c r="D43" s="5"/>
       <c r="F43" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="D44" s="5"/>
       <c r="F44" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>54</v>
@@ -1662,27 +1662,27 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D46" s="5"/>
       <c r="F46" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="D47" s="5"/>
       <c r="F47" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
@@ -1694,10 +1694,10 @@
       </c>
       <c r="D48" s="5"/>
       <c r="F48" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -1709,10 +1709,10 @@
       </c>
       <c r="D49" s="5"/>
       <c r="F49" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="D50" s="5"/>
       <c r="F50" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>54</v>
@@ -1790,10 +1790,10 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D59" s="5"/>
     </row>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D63" s="8"/>
     </row>
@@ -1845,10 +1845,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="5"/>
     </row>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D71" s="5"/>
     </row>
@@ -1983,7 +1983,7 @@
         <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
@@ -1991,7 +1991,7 @@
         <v>9</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D85" s="5"/>
     </row>
@@ -2016,10 +2016,10 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D89" s="5"/>
     </row>
@@ -2052,10 +2052,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D93" s="5"/>
     </row>
@@ -2293,10 +2293,10 @@
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C126" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D126" s="5"/>
     </row>
@@ -2329,10 +2329,10 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C130" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D130" s="5"/>
     </row>
@@ -2387,7 +2387,7 @@
         <v>5</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D137" s="5"/>
     </row>
@@ -2407,7 +2407,7 @@
         <v>9</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D139" s="5"/>
     </row>
@@ -2509,10 +2509,10 @@
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D153" s="5"/>
     </row>
@@ -2545,10 +2545,10 @@
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D157" s="5"/>
     </row>
@@ -2561,7 +2561,7 @@
         <v>5</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D159" s="5"/>
     </row>
@@ -2672,7 +2672,7 @@
         <v>5</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D174" s="5"/>
     </row>
@@ -2723,7 +2723,7 @@
         <v>12</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
@@ -2731,7 +2731,7 @@
         <v>9</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D181" s="5"/>
     </row>
@@ -2756,10 +2756,10 @@
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D185" s="5"/>
     </row>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D189" s="5"/>
     </row>
@@ -3040,10 +3040,10 @@
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C222" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D222" s="5"/>
     </row>
@@ -3076,10 +3076,10 @@
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C226" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D226" s="5"/>
     </row>
@@ -3211,10 +3211,10 @@
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D244" s="5"/>
     </row>
@@ -3247,10 +3247,10 @@
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D248" s="5"/>
     </row>
@@ -3414,7 +3414,7 @@
         <v>5</v>
       </c>
       <c r="C270" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D270" s="5"/>
     </row>
@@ -3457,10 +3457,10 @@
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C276" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D276" s="5"/>
     </row>
@@ -3493,10 +3493,10 @@
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C280" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D280" s="5"/>
     </row>
@@ -3509,7 +3509,7 @@
         <v>5</v>
       </c>
       <c r="C282" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D282" s="5"/>
     </row>
@@ -3591,10 +3591,10 @@
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C293" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D293" s="5"/>
     </row>
@@ -3627,10 +3627,10 @@
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C297" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D297" s="5"/>
     </row>
@@ -3725,10 +3725,10 @@
     </row>
     <row r="310" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B310" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C310" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D310" s="5"/>
     </row>
@@ -3746,7 +3746,7 @@
         <v>3</v>
       </c>
       <c r="C312" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D312" s="5"/>
     </row>
@@ -3761,10 +3761,10 @@
     </row>
     <row r="314" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B314" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C314" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D314" s="5"/>
     </row>
@@ -3848,16 +3848,16 @@
         <v>0</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D326" s="3"/>
     </row>
     <row r="327" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B327" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C327" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D327" s="5"/>
     </row>
@@ -3875,7 +3875,7 @@
         <v>3</v>
       </c>
       <c r="C329" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D329" s="5"/>
     </row>
@@ -3890,10 +3890,10 @@
     </row>
     <row r="331" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B331" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C331" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D331" s="5"/>
     </row>
@@ -3940,16 +3940,16 @@
         <v>0</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D338" s="3"/>
     </row>
     <row r="339" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B339" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C339" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D339" s="5"/>
     </row>
@@ -3967,7 +3967,7 @@
         <v>3</v>
       </c>
       <c r="C341" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D341" s="5"/>
     </row>
@@ -3982,10 +3982,10 @@
     </row>
     <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C343" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D343" s="5"/>
     </row>
@@ -4183,7 +4183,7 @@
         <v>5</v>
       </c>
       <c r="C370" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D370" s="5"/>
     </row>
@@ -4195,7 +4195,7 @@
         <v>41</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="372" spans="2:4" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
         <v>9</v>
       </c>
       <c r="C372" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D372" s="5"/>
     </row>
@@ -4225,7 +4225,7 @@
         <v>5</v>
       </c>
       <c r="C375" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D375" s="5"/>
     </row>
@@ -4262,7 +4262,7 @@
         <v>5</v>
       </c>
       <c r="C380" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D380" s="5"/>
     </row>
@@ -4274,7 +4274,7 @@
         <v>12</v>
       </c>
       <c r="D381" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="382" spans="2:4" x14ac:dyDescent="0.25">
@@ -4282,7 +4282,7 @@
         <v>9</v>
       </c>
       <c r="C382" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D382" s="5"/>
     </row>

</xml_diff>

<commit_message>
Updated building blocks and IMCS config to allow for Anji to test new IMCS elution parameters. Also found a bug in the notify script. Fixed.
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF081B-8AD8-4890-9A0C-86875D34AE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
     <sheet name="Colors" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -466,9 +460,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>MAM/Low Artifact,HCP/Proteomics,Anjis Elution method</t>
-  </si>
-  <si>
     <t>No,Dispense:10,Aspirate:10,Aspirate:10 + Dispense:10</t>
   </si>
   <si>
@@ -509,12 +500,15 @@
   </si>
   <si>
     <t>Max Dilution Steps</t>
+  </si>
+  <si>
+    <t>MAM/Low Artifact,HCP/Proteomics,Low Sample Elution,Corrected Sample Elution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -681,7 +675,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E92CFE-7DE1-496B-A04F-72766E21AE04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60E92CFE-7DE1-496B-A04F-72766E21AE04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -725,7 +719,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D708502C-F841-41C4-9DD7-9DA7291364AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D708502C-F841-41C4-9DD7-9DA7291364AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1043,19 +1037,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="C319" sqref="C319"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="F167" sqref="F167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,7 +1977,7 @@
         <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
@@ -2723,7 +2717,7 @@
         <v>12</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
@@ -3509,7 +3503,7 @@
         <v>5</v>
       </c>
       <c r="C282" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D282" s="5"/>
     </row>
@@ -3848,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D326" s="3"/>
     </row>
@@ -3875,7 +3869,7 @@
         <v>3</v>
       </c>
       <c r="C329" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D329" s="5"/>
     </row>
@@ -3893,7 +3887,7 @@
         <v>112</v>
       </c>
       <c r="C331" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D331" s="5"/>
     </row>
@@ -3940,7 +3934,7 @@
         <v>0</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D338" s="3"/>
     </row>
@@ -3967,7 +3961,7 @@
         <v>3</v>
       </c>
       <c r="C341" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D341" s="5"/>
     </row>
@@ -3985,7 +3979,7 @@
         <v>112</v>
       </c>
       <c r="C343" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D343" s="5"/>
     </row>
@@ -4183,7 +4177,7 @@
         <v>5</v>
       </c>
       <c r="C370" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D370" s="5"/>
     </row>
@@ -4195,7 +4189,7 @@
         <v>41</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="372" spans="2:4" x14ac:dyDescent="0.25">
@@ -4203,7 +4197,7 @@
         <v>9</v>
       </c>
       <c r="C372" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D372" s="5"/>
     </row>
@@ -4225,7 +4219,7 @@
         <v>5</v>
       </c>
       <c r="C375" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D375" s="5"/>
     </row>
@@ -4262,7 +4256,7 @@
         <v>5</v>
       </c>
       <c r="C380" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D380" s="5"/>
     </row>
@@ -4274,7 +4268,7 @@
         <v>12</v>
       </c>
       <c r="D381" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="382" spans="2:4" x14ac:dyDescent="0.25">
@@ -4282,7 +4276,7 @@
         <v>9</v>
       </c>
       <c r="C382" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D382" s="5"/>
     </row>
@@ -4301,7 +4295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0353A2-A6AC-4E44-A6E3-EA2FDBE0647A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Corrected Autoloading sequences for BioRad plates
</commit_message>
<xml_diff>
--- a/BuildingBlocks/BuildingBlocks.xlsx
+++ b/BuildingBlocks/BuildingBlocks.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonVisualMethodEditor\HamiltonVisualMethodEditorConfiguration\BuildingBlocks\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD30ECDE-C2AE-4B5F-9409-BC19B1F24D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BB502633-3274-4E6B-B4F6-5D789231924F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="BuildingBlocks" sheetId="1" r:id="rId1"/>
     <sheet name="Colors" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -283,9 +277,6 @@
     <t>100,100 + 100</t>
   </si>
   <si>
-    <t>96 Well PCR Plate,96 Well UV Plate</t>
-  </si>
-  <si>
     <t>MAM/Low Artifact</t>
   </si>
   <si>
@@ -509,12 +500,15 @@
   </si>
   <si>
     <t>Max Dilution Steps</t>
+  </si>
+  <si>
+    <t>96 Well PCR Plate,96 Well UV Plate,48 Well LC Vial Rack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -681,7 +675,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E92CFE-7DE1-496B-A04F-72766E21AE04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{60E92CFE-7DE1-496B-A04F-72766E21AE04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -725,7 +719,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D708502C-F841-41C4-9DD7-9DA7291364AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D708502C-F841-41C4-9DD7-9DA7291364AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1043,19 +1037,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C17CCE-D8C8-48DF-ACC4-969912519E9B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:G383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
-      <selection activeCell="C331" sqref="C331"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,23 +1074,23 @@
       </c>
       <c r="D2" s="3"/>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1108,7 +1102,7 @@
       </c>
       <c r="D4" s="5"/>
       <c r="F4" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>28</v>
@@ -1123,10 +1117,10 @@
       </c>
       <c r="D5" s="5"/>
       <c r="F5" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1138,35 +1132,35 @@
       </c>
       <c r="D6" s="5"/>
       <c r="F6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="5"/>
       <c r="F7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="D8" s="5"/>
       <c r="F8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1189,10 +1183,10 @@
       </c>
       <c r="D10" s="5"/>
       <c r="F10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1201,10 +1195,10 @@
       </c>
       <c r="D11" s="5"/>
       <c r="F11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
@@ -1216,20 +1210,20 @@
       </c>
       <c r="D12" s="5"/>
       <c r="F12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="D13" s="5"/>
       <c r="F13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1241,7 +1235,7 @@
       </c>
       <c r="D14" s="5"/>
       <c r="F14" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>54</v>
@@ -1255,7 +1249,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>82</v>
+        <v>157</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
@@ -1269,10 +1263,10 @@
       </c>
       <c r="D16" s="5"/>
       <c r="F16" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1284,18 +1278,18 @@
       </c>
       <c r="D17" s="8"/>
       <c r="F17" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1307,22 +1301,22 @@
       </c>
       <c r="D19" s="3"/>
       <c r="F19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D20" s="5"/>
       <c r="F20" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>54</v>
@@ -1348,10 +1342,10 @@
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1363,35 +1357,35 @@
       </c>
       <c r="D23" s="5"/>
       <c r="F23" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="D25" s="5"/>
       <c r="F25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1403,10 +1397,10 @@
       </c>
       <c r="D26" s="5"/>
       <c r="F26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -1417,7 +1411,7 @@
         <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
@@ -1428,10 +1422,10 @@
       </c>
       <c r="D28" s="5"/>
       <c r="F28" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1443,20 +1437,20 @@
       </c>
       <c r="D29" s="5"/>
       <c r="F29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="D30" s="5"/>
       <c r="F30" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1464,14 +1458,14 @@
         <v>5</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D31" s="5"/>
       <c r="F31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -1483,7 +1477,7 @@
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>54</v>
@@ -1509,20 +1503,20 @@
       </c>
       <c r="D34" s="5"/>
       <c r="F34" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="D35" s="5"/>
       <c r="F35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -1530,14 +1524,14 @@
         <v>5</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" s="5"/>
       <c r="F36" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -1549,10 +1543,10 @@
       </c>
       <c r="D37" s="5"/>
       <c r="F37" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -1564,7 +1558,7 @@
       </c>
       <c r="D38" s="5"/>
       <c r="F38" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>54</v>
@@ -1583,10 +1577,10 @@
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F40" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -1598,25 +1592,25 @@
       </c>
       <c r="D41" s="3"/>
       <c r="F41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D42" s="5"/>
       <c r="F42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -1628,10 +1622,10 @@
       </c>
       <c r="D43" s="5"/>
       <c r="F43" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
@@ -1643,7 +1637,7 @@
       </c>
       <c r="D44" s="5"/>
       <c r="F44" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>54</v>
@@ -1662,27 +1656,27 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D46" s="5"/>
       <c r="F46" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="4"/>
       <c r="D47" s="5"/>
       <c r="F47" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
@@ -1694,10 +1688,10 @@
       </c>
       <c r="D48" s="5"/>
       <c r="F48" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -1709,10 +1703,10 @@
       </c>
       <c r="D49" s="5"/>
       <c r="F49" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1721,7 +1715,7 @@
       </c>
       <c r="D50" s="5"/>
       <c r="F50" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>54</v>
@@ -1790,10 +1784,10 @@
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D59" s="5"/>
     </row>
@@ -1826,10 +1820,10 @@
     </row>
     <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D63" s="8"/>
     </row>
@@ -1845,10 +1839,10 @@
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D67" s="5"/>
     </row>
@@ -1881,10 +1875,10 @@
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D71" s="5"/>
     </row>
@@ -1983,7 +1977,7 @@
         <v>41</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
@@ -1991,7 +1985,7 @@
         <v>9</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D85" s="5"/>
     </row>
@@ -2016,10 +2010,10 @@
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D89" s="5"/>
     </row>
@@ -2052,10 +2046,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D93" s="5"/>
     </row>
@@ -2293,10 +2287,10 @@
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C126" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D126" s="5"/>
     </row>
@@ -2329,10 +2323,10 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C130" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D130" s="5"/>
     </row>
@@ -2387,7 +2381,7 @@
         <v>5</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D137" s="5"/>
     </row>
@@ -2407,7 +2401,7 @@
         <v>9</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D139" s="5"/>
     </row>
@@ -2509,10 +2503,10 @@
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D153" s="5"/>
     </row>
@@ -2545,10 +2539,10 @@
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D157" s="5"/>
     </row>
@@ -2561,7 +2555,7 @@
         <v>5</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D159" s="5"/>
     </row>
@@ -2672,7 +2666,7 @@
         <v>5</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D174" s="5"/>
     </row>
@@ -2723,7 +2717,7 @@
         <v>12</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
@@ -2731,7 +2725,7 @@
         <v>9</v>
       </c>
       <c r="C181" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D181" s="5"/>
     </row>
@@ -2756,10 +2750,10 @@
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C185" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D185" s="5"/>
     </row>
@@ -2792,10 +2786,10 @@
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C189" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D189" s="5"/>
     </row>
@@ -3040,10 +3034,10 @@
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B222" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C222" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D222" s="5"/>
     </row>
@@ -3076,10 +3070,10 @@
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B226" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C226" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D226" s="5"/>
     </row>
@@ -3211,10 +3205,10 @@
     </row>
     <row r="244" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B244" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C244" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D244" s="5"/>
     </row>
@@ -3247,10 +3241,10 @@
     </row>
     <row r="248" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B248" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C248" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D248" s="5"/>
     </row>
@@ -3414,7 +3408,7 @@
         <v>5</v>
       </c>
       <c r="C270" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D270" s="5"/>
     </row>
@@ -3457,10 +3451,10 @@
     </row>
     <row r="276" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B276" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C276" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D276" s="5"/>
     </row>
@@ -3493,10 +3487,10 @@
     </row>
     <row r="280" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B280" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C280" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D280" s="5"/>
     </row>
@@ -3509,7 +3503,7 @@
         <v>5</v>
       </c>
       <c r="C282" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D282" s="5"/>
     </row>
@@ -3591,10 +3585,10 @@
     </row>
     <row r="293" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B293" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C293" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D293" s="5"/>
     </row>
@@ -3627,10 +3621,10 @@
     </row>
     <row r="297" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B297" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C297" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D297" s="5"/>
     </row>
@@ -3725,10 +3719,10 @@
     </row>
     <row r="310" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B310" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C310" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D310" s="5"/>
     </row>
@@ -3746,7 +3740,7 @@
         <v>3</v>
       </c>
       <c r="C312" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D312" s="5"/>
     </row>
@@ -3761,10 +3755,10 @@
     </row>
     <row r="314" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B314" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C314" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D314" s="5"/>
     </row>
@@ -3848,16 +3842,16 @@
         <v>0</v>
       </c>
       <c r="C326" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D326" s="3"/>
     </row>
     <row r="327" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B327" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C327" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D327" s="5"/>
     </row>
@@ -3875,7 +3869,7 @@
         <v>3</v>
       </c>
       <c r="C329" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D329" s="5"/>
     </row>
@@ -3890,10 +3884,10 @@
     </row>
     <row r="331" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B331" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C331" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D331" s="5"/>
     </row>
@@ -3940,16 +3934,16 @@
         <v>0</v>
       </c>
       <c r="C338" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D338" s="3"/>
     </row>
     <row r="339" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B339" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C339" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D339" s="5"/>
     </row>
@@ -3967,7 +3961,7 @@
         <v>3</v>
       </c>
       <c r="C341" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D341" s="5"/>
     </row>
@@ -3982,10 +3976,10 @@
     </row>
     <row r="343" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B343" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C343" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D343" s="5"/>
     </row>
@@ -4183,7 +4177,7 @@
         <v>5</v>
       </c>
       <c r="C370" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D370" s="5"/>
     </row>
@@ -4195,7 +4189,7 @@
         <v>41</v>
       </c>
       <c r="D371" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="372" spans="2:4" x14ac:dyDescent="0.25">
@@ -4203,7 +4197,7 @@
         <v>9</v>
       </c>
       <c r="C372" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D372" s="5"/>
     </row>
@@ -4225,7 +4219,7 @@
         <v>5</v>
       </c>
       <c r="C375" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D375" s="5"/>
     </row>
@@ -4262,7 +4256,7 @@
         <v>5</v>
       </c>
       <c r="C380" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D380" s="5"/>
     </row>
@@ -4274,7 +4268,7 @@
         <v>12</v>
       </c>
       <c r="D381" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="382" spans="2:4" x14ac:dyDescent="0.25">
@@ -4282,7 +4276,7 @@
         <v>9</v>
       </c>
       <c r="C382" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D382" s="5"/>
     </row>
@@ -4301,7 +4295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0353A2-A6AC-4E44-A6E3-EA2FDBE0647A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>